<commit_message>
Volume issues were solved.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" firstSheet="2" activeTab="2" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
     <sheet name="TIPO_EVENTO" sheetId="3" r:id="rId2"/>
     <sheet name="TIPO_PRODUCTO" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -1220,10 +1220,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5719,8 +5719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Books chapters were added.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C317F9B9-19BB-4CE1-A469-FAA0B6604919}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" activeTab="1" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="173">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -534,6 +533,18 @@
   </si>
   <si>
     <t>Libro - pedagógico</t>
+  </si>
+  <si>
+    <t>Otro capítulo de libro publicado</t>
+  </si>
+  <si>
+    <t>Capítulo de libro</t>
+  </si>
+  <si>
+    <t>Capítulo de libro - Otro</t>
+  </si>
+  <si>
+    <t>Otro capítulo de libro</t>
   </si>
 </sst>
 </file>
@@ -1250,11 +1261,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70E6F07-A587-464B-AE84-05F19DCFB741}">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="G51" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M68" sqref="M60:M68"/>
+      <selection pane="bottomRight" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1458,7 @@
       <c r="M3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O3" s="14" t="s">
@@ -1544,7 +1555,7 @@
       <c r="M4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O4" s="14" t="s">
@@ -1641,7 +1652,7 @@
       <c r="M5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O5" s="14" t="s">
@@ -1734,7 +1745,7 @@
       <c r="M6" s="26">
         <v>3</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="26">
         <v>4</v>
       </c>
       <c r="O6" s="14">
@@ -1819,7 +1830,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
-      <c r="N7" s="14"/>
+      <c r="N7" s="26"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -1862,7 +1873,7 @@
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
-      <c r="N8" s="14"/>
+      <c r="N8" s="26"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -1907,7 +1918,7 @@
       <c r="K9" s="26"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
-      <c r="N9" s="14"/>
+      <c r="N9" s="26"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -1956,7 +1967,7 @@
       <c r="M10" s="26">
         <v>4</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="26">
         <v>5</v>
       </c>
       <c r="O10" s="14">
@@ -2043,7 +2054,7 @@
       <c r="M11" s="26">
         <v>5</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="26">
         <v>12</v>
       </c>
       <c r="O11" s="14">
@@ -2126,7 +2137,7 @@
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
-      <c r="N12" s="14"/>
+      <c r="N12" s="26"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -2169,7 +2180,7 @@
       <c r="M13" s="26">
         <v>10</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="26">
         <v>13</v>
       </c>
       <c r="O13" s="14">
@@ -2248,7 +2259,7 @@
       <c r="M14" s="26">
         <v>11</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="26">
         <v>14</v>
       </c>
       <c r="O14" s="14">
@@ -2325,7 +2336,7 @@
       <c r="M15" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="26">
         <v>15</v>
       </c>
       <c r="O15" s="14"/>
@@ -2402,7 +2413,7 @@
       <c r="M16" s="26">
         <v>2</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="26">
         <v>2</v>
       </c>
       <c r="O16" s="14">
@@ -2483,7 +2494,7 @@
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
-      <c r="N17" s="14"/>
+      <c r="N17" s="26"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -2528,7 +2539,7 @@
       <c r="M18" s="26">
         <v>6</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18" s="26">
         <v>7</v>
       </c>
       <c r="O18" s="14"/>
@@ -2579,7 +2590,7 @@
       <c r="M19" s="26">
         <v>8</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="26">
         <v>8</v>
       </c>
       <c r="O19" s="14">
@@ -2628,7 +2639,7 @@
       <c r="M20" s="26">
         <v>9</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="26">
         <v>11</v>
       </c>
       <c r="O20" s="14"/>
@@ -2683,7 +2694,7 @@
         <v>13</v>
       </c>
       <c r="M21" s="26"/>
-      <c r="N21" s="14"/>
+      <c r="N21" s="26"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -2724,7 +2735,7 @@
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
-      <c r="N22" s="14"/>
+      <c r="N22" s="26"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -2773,7 +2784,7 @@
       <c r="K23" s="26"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
-      <c r="N23" s="14"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -2816,7 +2827,7 @@
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
-      <c r="N24" s="14"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -2864,7 +2875,7 @@
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
-      <c r="N26" s="14"/>
+      <c r="N26" s="27"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -2909,7 +2920,7 @@
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
@@ -2952,7 +2963,7 @@
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
       <c r="M28" s="27"/>
-      <c r="N28" s="14"/>
+      <c r="N28" s="27"/>
       <c r="O28" s="14"/>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
@@ -2995,7 +3006,7 @@
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
-      <c r="N29" s="14"/>
+      <c r="N29" s="27"/>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
@@ -3038,7 +3049,7 @@
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
-      <c r="N30" s="14"/>
+      <c r="N30" s="27"/>
       <c r="O30" s="14"/>
       <c r="P30" s="14"/>
       <c r="Q30" s="14"/>
@@ -3081,7 +3092,7 @@
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
-      <c r="N31" s="14"/>
+      <c r="N31" s="27"/>
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
@@ -3130,7 +3141,7 @@
       <c r="K33" s="27"/>
       <c r="L33" s="27"/>
       <c r="M33" s="27"/>
-      <c r="N33" s="14"/>
+      <c r="N33" s="27"/>
       <c r="O33" s="14"/>
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
@@ -3177,7 +3188,7 @@
       <c r="K34" s="27"/>
       <c r="L34" s="27"/>
       <c r="M34" s="27"/>
-      <c r="N34" s="14"/>
+      <c r="N34" s="27"/>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
       <c r="Q34" s="14"/>
@@ -3220,7 +3231,7 @@
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
-      <c r="N35" s="14"/>
+      <c r="N35" s="27"/>
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
       <c r="Q35" s="14"/>
@@ -3263,7 +3274,7 @@
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
-      <c r="N36" s="14"/>
+      <c r="N36" s="27"/>
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
       <c r="Q36" s="14"/>
@@ -3306,7 +3317,7 @@
       <c r="K37" s="27"/>
       <c r="L37" s="27"/>
       <c r="M37" s="27"/>
-      <c r="N37" s="14"/>
+      <c r="N37" s="27"/>
       <c r="O37" s="14"/>
       <c r="P37" s="14"/>
       <c r="Q37" s="14"/>
@@ -3349,7 +3360,7 @@
       <c r="K38" s="27"/>
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
-      <c r="N38" s="14"/>
+      <c r="N38" s="27"/>
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
@@ -3410,7 +3421,7 @@
       <c r="M40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O40" s="14" t="s">
@@ -3509,7 +3520,7 @@
       <c r="M41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N41" s="14" t="s">
+      <c r="N41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O41" s="14" t="s">
@@ -3600,7 +3611,7 @@
       <c r="M42" s="26">
         <v>1</v>
       </c>
-      <c r="N42" s="14">
+      <c r="N42" s="26">
         <v>1</v>
       </c>
       <c r="O42" s="14">
@@ -3677,7 +3688,7 @@
       <c r="K43" s="26"/>
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
-      <c r="N43" s="14"/>
+      <c r="N43" s="26"/>
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
@@ -3718,7 +3729,7 @@
       <c r="K44" s="26"/>
       <c r="L44" s="26"/>
       <c r="M44" s="26"/>
-      <c r="N44" s="14"/>
+      <c r="N44" s="26"/>
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
       <c r="Q44" s="14"/>
@@ -3759,7 +3770,7 @@
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
-      <c r="N45" s="14"/>
+      <c r="N45" s="26"/>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
@@ -3810,7 +3821,7 @@
       </c>
       <c r="L47" s="27"/>
       <c r="M47" s="27"/>
-      <c r="N47" s="14"/>
+      <c r="N47" s="27"/>
       <c r="O47" s="14"/>
       <c r="P47" s="14"/>
       <c r="Q47" s="14"/>
@@ -3859,7 +3870,7 @@
       </c>
       <c r="L48" s="27"/>
       <c r="M48" s="27"/>
-      <c r="N48" s="14"/>
+      <c r="N48" s="27"/>
       <c r="O48" s="14"/>
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
@@ -3906,7 +3917,7 @@
       </c>
       <c r="L49" s="27"/>
       <c r="M49" s="27"/>
-      <c r="N49" s="14"/>
+      <c r="N49" s="27"/>
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
       <c r="Q49" s="14"/>
@@ -3953,7 +3964,7 @@
       </c>
       <c r="L50" s="27"/>
       <c r="M50" s="27"/>
-      <c r="N50" s="14"/>
+      <c r="N50" s="27"/>
       <c r="O50" s="14"/>
       <c r="P50" s="14"/>
       <c r="Q50" s="14"/>
@@ -4000,7 +4011,7 @@
       </c>
       <c r="L51" s="27"/>
       <c r="M51" s="27"/>
-      <c r="N51" s="14"/>
+      <c r="N51" s="27"/>
       <c r="O51" s="14"/>
       <c r="P51" s="14"/>
       <c r="Q51" s="14"/>
@@ -4047,7 +4058,7 @@
       </c>
       <c r="L52" s="27"/>
       <c r="M52" s="27"/>
-      <c r="N52" s="14"/>
+      <c r="N52" s="27"/>
       <c r="O52" s="14"/>
       <c r="P52" s="14"/>
       <c r="Q52" s="14"/>
@@ -4094,7 +4105,7 @@
       </c>
       <c r="L53" s="27"/>
       <c r="M53" s="27"/>
-      <c r="N53" s="14"/>
+      <c r="N53" s="27"/>
       <c r="O53" s="14"/>
       <c r="P53" s="14"/>
       <c r="Q53" s="14"/>
@@ -4141,7 +4152,7 @@
       </c>
       <c r="L54" s="27"/>
       <c r="M54" s="27"/>
-      <c r="N54" s="14"/>
+      <c r="N54" s="27"/>
       <c r="O54" s="14"/>
       <c r="P54" s="14"/>
       <c r="Q54" s="14"/>
@@ -4190,7 +4201,7 @@
       <c r="M56" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N56" s="14" t="s">
+      <c r="N56" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O56" s="14" t="s">
@@ -4247,7 +4258,7 @@
       <c r="M57" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="N57" s="14" t="s">
+      <c r="N57" s="26" t="s">
         <v>55</v>
       </c>
       <c r="O57" s="14" t="s">
@@ -4300,7 +4311,7 @@
         <v>5</v>
       </c>
       <c r="M58" s="26"/>
-      <c r="N58" s="14"/>
+      <c r="N58" s="26"/>
       <c r="O58" s="14">
         <v>6</v>
       </c>
@@ -4347,7 +4358,7 @@
       <c r="M59" s="26">
         <v>7</v>
       </c>
-      <c r="N59" s="14"/>
+      <c r="N59" s="26"/>
       <c r="O59" s="14">
         <v>7</v>
       </c>
@@ -4390,7 +4401,7 @@
       <c r="K60" s="27"/>
       <c r="L60" s="26"/>
       <c r="M60" s="26"/>
-      <c r="N60" s="14"/>
+      <c r="N60" s="26"/>
       <c r="O60" s="14"/>
       <c r="P60" s="14"/>
       <c r="Q60" s="14">
@@ -4433,7 +4444,7 @@
       <c r="K61" s="27"/>
       <c r="L61" s="26"/>
       <c r="M61" s="26"/>
-      <c r="N61" s="14"/>
+      <c r="N61" s="26"/>
       <c r="O61" s="14"/>
       <c r="P61" s="14"/>
       <c r="Q61" s="14">
@@ -4476,7 +4487,7 @@
       <c r="K62" s="27"/>
       <c r="L62" s="26"/>
       <c r="M62" s="26"/>
-      <c r="N62" s="14"/>
+      <c r="N62" s="26"/>
       <c r="O62" s="14"/>
       <c r="P62" s="14"/>
       <c r="Q62" s="14">
@@ -4519,7 +4530,7 @@
       <c r="K63" s="27"/>
       <c r="L63" s="26"/>
       <c r="M63" s="26"/>
-      <c r="N63" s="14"/>
+      <c r="N63" s="26"/>
       <c r="O63" s="14"/>
       <c r="P63" s="14"/>
       <c r="Q63" s="14">
@@ -4562,7 +4573,7 @@
       <c r="K64" s="27"/>
       <c r="L64" s="26"/>
       <c r="M64" s="26"/>
-      <c r="N64" s="14"/>
+      <c r="N64" s="26"/>
       <c r="O64" s="14"/>
       <c r="P64" s="14"/>
       <c r="Q64" s="14">
@@ -4605,7 +4616,7 @@
       <c r="K65" s="27"/>
       <c r="L65" s="26"/>
       <c r="M65" s="26"/>
-      <c r="N65" s="14">
+      <c r="N65" s="26">
         <v>3</v>
       </c>
       <c r="O65" s="14"/>
@@ -4650,7 +4661,7 @@
         <v>9</v>
       </c>
       <c r="M66" s="26"/>
-      <c r="N66" s="14"/>
+      <c r="N66" s="26"/>
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
       <c r="Q66" s="14">
@@ -4695,7 +4706,7 @@
         <v>10</v>
       </c>
       <c r="M67" s="26"/>
-      <c r="N67" s="14">
+      <c r="N67" s="26">
         <v>9</v>
       </c>
       <c r="O67" s="14">
@@ -4742,7 +4753,7 @@
         <v>11</v>
       </c>
       <c r="M68" s="26"/>
-      <c r="N68" s="14">
+      <c r="N68" s="26">
         <v>10</v>
       </c>
       <c r="O68" s="14">
@@ -4789,7 +4800,7 @@
       <c r="K70" s="27"/>
       <c r="L70" s="27"/>
       <c r="M70" s="27"/>
-      <c r="N70" s="14"/>
+      <c r="N70" s="27"/>
       <c r="O70" s="14"/>
       <c r="P70" s="14"/>
       <c r="Q70" s="14"/>
@@ -4860,7 +4871,7 @@
       <c r="K71" s="27"/>
       <c r="L71" s="27"/>
       <c r="M71" s="27"/>
-      <c r="N71" s="14"/>
+      <c r="N71" s="27"/>
       <c r="O71" s="14"/>
       <c r="P71" s="14"/>
       <c r="Q71" s="14"/>
@@ -4931,7 +4942,7 @@
       <c r="K72" s="27"/>
       <c r="L72" s="27"/>
       <c r="M72" s="27"/>
-      <c r="N72" s="14"/>
+      <c r="N72" s="27"/>
       <c r="O72" s="14"/>
       <c r="P72" s="14"/>
       <c r="Q72" s="14"/>
@@ -4996,7 +5007,7 @@
       <c r="K73" s="27"/>
       <c r="L73" s="27"/>
       <c r="M73" s="27"/>
-      <c r="N73" s="14"/>
+      <c r="N73" s="27"/>
       <c r="O73" s="14"/>
       <c r="P73" s="14"/>
       <c r="Q73" s="14"/>
@@ -5065,7 +5076,7 @@
       <c r="K74" s="27"/>
       <c r="L74" s="27"/>
       <c r="M74" s="27"/>
-      <c r="N74" s="14"/>
+      <c r="N74" s="27"/>
       <c r="O74" s="14"/>
       <c r="P74" s="14"/>
       <c r="Q74" s="14"/>
@@ -5108,7 +5119,7 @@
       <c r="K75" s="27"/>
       <c r="L75" s="27"/>
       <c r="M75" s="27"/>
-      <c r="N75" s="14"/>
+      <c r="N75" s="27"/>
       <c r="O75" s="14"/>
       <c r="P75" s="14"/>
       <c r="Q75" s="14"/>
@@ -5155,7 +5166,7 @@
       <c r="K76" s="27"/>
       <c r="L76" s="27"/>
       <c r="M76" s="27"/>
-      <c r="N76" s="14"/>
+      <c r="N76" s="27"/>
       <c r="O76" s="14"/>
       <c r="P76" s="14"/>
       <c r="Q76" s="14"/>
@@ -5200,7 +5211,7 @@
       <c r="K77" s="27"/>
       <c r="L77" s="27"/>
       <c r="M77" s="27"/>
-      <c r="N77" s="14"/>
+      <c r="N77" s="27"/>
       <c r="O77" s="14"/>
       <c r="P77" s="14"/>
       <c r="Q77" s="14"/>
@@ -5245,7 +5256,7 @@
       <c r="K78" s="27"/>
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
-      <c r="N78" s="14"/>
+      <c r="N78" s="27"/>
       <c r="O78" s="14"/>
       <c r="P78" s="14"/>
       <c r="Q78" s="14"/>
@@ -5288,7 +5299,7 @@
       <c r="K79" s="27"/>
       <c r="L79" s="27"/>
       <c r="M79" s="27"/>
-      <c r="N79" s="14"/>
+      <c r="N79" s="27"/>
       <c r="O79" s="14"/>
       <c r="P79" s="14"/>
       <c r="Q79" s="14"/>
@@ -5331,7 +5342,7 @@
       <c r="K80" s="27"/>
       <c r="L80" s="27"/>
       <c r="M80" s="27"/>
-      <c r="N80" s="14"/>
+      <c r="N80" s="27"/>
       <c r="O80" s="14"/>
       <c r="P80" s="14"/>
       <c r="Q80" s="14"/>
@@ -5374,7 +5385,7 @@
       <c r="K81" s="27"/>
       <c r="L81" s="27"/>
       <c r="M81" s="27"/>
-      <c r="N81" s="14"/>
+      <c r="N81" s="27"/>
       <c r="O81" s="14"/>
       <c r="P81" s="14"/>
       <c r="Q81" s="14"/>
@@ -5423,7 +5434,7 @@
       <c r="K83" s="27"/>
       <c r="L83" s="27"/>
       <c r="M83" s="27"/>
-      <c r="N83" s="14"/>
+      <c r="N83" s="27"/>
       <c r="O83" s="14"/>
       <c r="P83" s="14"/>
       <c r="Q83" s="14"/>
@@ -5468,7 +5479,7 @@
       <c r="K84" s="27"/>
       <c r="L84" s="27"/>
       <c r="M84" s="27"/>
-      <c r="N84" s="14"/>
+      <c r="N84" s="27"/>
       <c r="O84" s="14"/>
       <c r="P84" s="14"/>
       <c r="Q84" s="14"/>
@@ -5509,7 +5520,7 @@
       <c r="K85" s="27"/>
       <c r="L85" s="27"/>
       <c r="M85" s="27"/>
-      <c r="N85" s="14"/>
+      <c r="N85" s="27"/>
       <c r="O85" s="14"/>
       <c r="P85" s="14"/>
       <c r="Q85" s="14"/>
@@ -5550,7 +5561,7 @@
       <c r="K86" s="27"/>
       <c r="L86" s="27"/>
       <c r="M86" s="27"/>
-      <c r="N86" s="14"/>
+      <c r="N86" s="27"/>
       <c r="O86" s="14"/>
       <c r="P86" s="14"/>
       <c r="Q86" s="14"/>
@@ -5591,7 +5602,7 @@
       <c r="K87" s="27"/>
       <c r="L87" s="27"/>
       <c r="M87" s="27"/>
-      <c r="N87" s="14"/>
+      <c r="N87" s="27"/>
       <c r="O87" s="14"/>
       <c r="P87" s="14"/>
       <c r="Q87" s="14"/>
@@ -5634,10 +5645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5950,6 +5961,34 @@
       </c>
       <c r="D21" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not Scientific Texts were Added.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="183">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -545,6 +545,36 @@
   </si>
   <si>
     <t>Otro capítulo de libro</t>
+  </si>
+  <si>
+    <t>Periódico de noticias</t>
+  </si>
+  <si>
+    <t>Revista de divulgación</t>
+  </si>
+  <si>
+    <t>Cartas al editor</t>
+  </si>
+  <si>
+    <t>Reseñas de libros</t>
+  </si>
+  <si>
+    <t>Columnas de opinión</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otro artículo publicado - Periódico de noticias</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otro artículo publicado - Revista de divulgación</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otro artículo publicado - Cartas al editor</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otro artículo publicado - Reseñas de libros</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otro artículo publicado - Columnas de opinión</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1292,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="L57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N41" sqref="N41"/>
+      <selection pane="bottomRight" activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1491,7 @@
       <c r="N3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P3" s="14" t="s">
@@ -1558,7 +1588,7 @@
       <c r="N4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P4" s="14" t="s">
@@ -1655,7 +1685,7 @@
       <c r="N5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P5" s="14" t="s">
@@ -1748,7 +1778,7 @@
       <c r="N6" s="26">
         <v>4</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="26">
         <v>3</v>
       </c>
       <c r="P6" s="14">
@@ -1831,7 +1861,7 @@
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
-      <c r="O7" s="14"/>
+      <c r="O7" s="26"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
@@ -1874,7 +1904,7 @@
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
-      <c r="O8" s="14"/>
+      <c r="O8" s="26"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
@@ -1919,7 +1949,7 @@
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="14"/>
+      <c r="O9" s="26"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
@@ -1970,7 +2000,7 @@
       <c r="N10" s="26">
         <v>5</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="26">
         <v>4</v>
       </c>
       <c r="P10" s="14">
@@ -2057,7 +2087,7 @@
       <c r="N11" s="26">
         <v>12</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="26">
         <v>5</v>
       </c>
       <c r="P11" s="14">
@@ -2138,7 +2168,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
-      <c r="O12" s="14"/>
+      <c r="O12" s="26"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
@@ -2183,7 +2213,7 @@
       <c r="N13" s="26">
         <v>13</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="26">
         <v>11</v>
       </c>
       <c r="P13" s="14">
@@ -2262,7 +2292,7 @@
       <c r="N14" s="26">
         <v>14</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="26">
         <v>12</v>
       </c>
       <c r="P14" s="14"/>
@@ -2339,7 +2369,7 @@
       <c r="N15" s="26">
         <v>15</v>
       </c>
-      <c r="O15" s="14"/>
+      <c r="O15" s="26"/>
       <c r="P15" s="14">
         <v>8</v>
       </c>
@@ -2416,7 +2446,7 @@
       <c r="N16" s="26">
         <v>2</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16" s="26">
         <v>2</v>
       </c>
       <c r="P16" s="14">
@@ -2495,7 +2525,7 @@
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
-      <c r="O17" s="14"/>
+      <c r="O17" s="26"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
@@ -2542,7 +2572,7 @@
       <c r="N18" s="26">
         <v>7</v>
       </c>
-      <c r="O18" s="14"/>
+      <c r="O18" s="26"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
@@ -2593,7 +2623,7 @@
       <c r="N19" s="26">
         <v>8</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="26">
         <v>12</v>
       </c>
       <c r="P19" s="14"/>
@@ -2642,7 +2672,7 @@
       <c r="N20" s="26">
         <v>11</v>
       </c>
-      <c r="O20" s="14"/>
+      <c r="O20" s="26"/>
       <c r="P20" s="14">
         <v>6</v>
       </c>
@@ -2695,7 +2725,7 @@
       </c>
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
-      <c r="O21" s="14"/>
+      <c r="O21" s="26"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
@@ -2736,7 +2766,7 @@
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
-      <c r="O22" s="14"/>
+      <c r="O22" s="26"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14"/>
@@ -2785,7 +2815,7 @@
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
-      <c r="O23" s="14"/>
+      <c r="O23" s="26"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
@@ -2828,7 +2858,7 @@
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
-      <c r="O24" s="14"/>
+      <c r="O24" s="26"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
@@ -3424,7 +3454,7 @@
       <c r="N40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O40" s="14" t="s">
+      <c r="O40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P40" s="14" t="s">
@@ -3523,7 +3553,7 @@
       <c r="N41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O41" s="14" t="s">
+      <c r="O41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P41" s="14" t="s">
@@ -3614,7 +3644,7 @@
       <c r="N42" s="26">
         <v>1</v>
       </c>
-      <c r="O42" s="14">
+      <c r="O42" s="26">
         <v>1</v>
       </c>
       <c r="P42" s="14">
@@ -3689,7 +3719,7 @@
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
       <c r="N43" s="26"/>
-      <c r="O43" s="14"/>
+      <c r="O43" s="26"/>
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
@@ -3730,7 +3760,7 @@
       <c r="L44" s="26"/>
       <c r="M44" s="26"/>
       <c r="N44" s="26"/>
-      <c r="O44" s="14"/>
+      <c r="O44" s="26"/>
       <c r="P44" s="14"/>
       <c r="Q44" s="14"/>
       <c r="R44" s="14"/>
@@ -3771,7 +3801,7 @@
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
       <c r="N45" s="26"/>
-      <c r="O45" s="14"/>
+      <c r="O45" s="26"/>
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
       <c r="R45" s="14"/>
@@ -4204,7 +4234,7 @@
       <c r="N56" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O56" s="14" t="s">
+      <c r="O56" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P56" s="14" t="s">
@@ -4261,7 +4291,7 @@
       <c r="N57" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="O57" s="14" t="s">
+      <c r="O57" s="26" t="s">
         <v>55</v>
       </c>
       <c r="P57" s="14" t="s">
@@ -4402,7 +4432,7 @@
       <c r="L60" s="26"/>
       <c r="M60" s="26"/>
       <c r="N60" s="26"/>
-      <c r="O60" s="14"/>
+      <c r="O60" s="26"/>
       <c r="P60" s="14"/>
       <c r="Q60" s="14">
         <v>6</v>
@@ -4445,7 +4475,7 @@
       <c r="L61" s="26"/>
       <c r="M61" s="26"/>
       <c r="N61" s="26"/>
-      <c r="O61" s="14"/>
+      <c r="O61" s="26"/>
       <c r="P61" s="14"/>
       <c r="Q61" s="14">
         <v>10</v>
@@ -4488,7 +4518,7 @@
       <c r="L62" s="26"/>
       <c r="M62" s="26"/>
       <c r="N62" s="26"/>
-      <c r="O62" s="14"/>
+      <c r="O62" s="26"/>
       <c r="P62" s="14"/>
       <c r="Q62" s="14">
         <v>9</v>
@@ -4531,7 +4561,7 @@
       <c r="L63" s="26"/>
       <c r="M63" s="26"/>
       <c r="N63" s="26"/>
-      <c r="O63" s="14"/>
+      <c r="O63" s="26"/>
       <c r="P63" s="14"/>
       <c r="Q63" s="14">
         <v>7</v>
@@ -4574,7 +4604,7 @@
       <c r="L64" s="26"/>
       <c r="M64" s="26"/>
       <c r="N64" s="26"/>
-      <c r="O64" s="14"/>
+      <c r="O64" s="26"/>
       <c r="P64" s="14"/>
       <c r="Q64" s="14">
         <v>8</v>
@@ -4619,7 +4649,7 @@
       <c r="N65" s="26">
         <v>3</v>
       </c>
-      <c r="O65" s="14"/>
+      <c r="O65" s="26"/>
       <c r="P65" s="14"/>
       <c r="Q65" s="14"/>
       <c r="R65" s="14"/>
@@ -4662,7 +4692,7 @@
       </c>
       <c r="M66" s="26"/>
       <c r="N66" s="26"/>
-      <c r="O66" s="14"/>
+      <c r="O66" s="26"/>
       <c r="P66" s="14"/>
       <c r="Q66" s="14">
         <v>11</v>
@@ -4709,7 +4739,7 @@
       <c r="N67" s="26">
         <v>9</v>
       </c>
-      <c r="O67" s="14">
+      <c r="O67" s="26">
         <v>8</v>
       </c>
       <c r="P67" s="14"/>
@@ -4756,7 +4786,7 @@
       <c r="N68" s="26">
         <v>10</v>
       </c>
-      <c r="O68" s="14">
+      <c r="O68" s="26">
         <v>9</v>
       </c>
       <c r="P68" s="14"/>
@@ -5645,10 +5675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5989,6 +6019,76 @@
       </c>
       <c r="D23" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working Pappers were added.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="185">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -575,6 +575,12 @@
   </si>
   <si>
     <t>Producción bibliográfica - Otro artículo publicado - Columnas de opinión</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Documento de trabajo (Working Paper)</t>
+  </si>
+  <si>
+    <t>Documento de trabajo (Working Paper)</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1298,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="L57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O58" sqref="O58"/>
+      <selection pane="bottomRight" activeCell="P31" sqref="P26:P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1500,7 @@
       <c r="O3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q3" s="14" t="s">
@@ -1591,7 +1597,7 @@
       <c r="O4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q4" s="14" t="s">
@@ -1688,7 +1694,7 @@
       <c r="O5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q5" s="14" t="s">
@@ -1781,7 +1787,7 @@
       <c r="O6" s="26">
         <v>3</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="26">
         <v>3</v>
       </c>
       <c r="Q6" s="14">
@@ -1862,7 +1868,7 @@
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
       <c r="O7" s="26"/>
-      <c r="P7" s="14"/>
+      <c r="P7" s="26"/>
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
@@ -1905,7 +1911,7 @@
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
-      <c r="P8" s="14"/>
+      <c r="P8" s="26"/>
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
@@ -1950,7 +1956,7 @@
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
       <c r="O9" s="26"/>
-      <c r="P9" s="14"/>
+      <c r="P9" s="26"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
       <c r="S9" s="14"/>
@@ -2003,7 +2009,7 @@
       <c r="O10" s="26">
         <v>4</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="26">
         <v>4</v>
       </c>
       <c r="Q10" s="14">
@@ -2090,7 +2096,7 @@
       <c r="O11" s="26">
         <v>5</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="26">
         <v>5</v>
       </c>
       <c r="Q11" s="14">
@@ -2169,7 +2175,7 @@
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
-      <c r="P12" s="14"/>
+      <c r="P12" s="26"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
@@ -2216,7 +2222,7 @@
       <c r="O13" s="26">
         <v>11</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="26">
         <v>7</v>
       </c>
       <c r="Q13" s="14">
@@ -2295,7 +2301,7 @@
       <c r="O14" s="26">
         <v>12</v>
       </c>
-      <c r="P14" s="14"/>
+      <c r="P14" s="26"/>
       <c r="Q14" s="14">
         <v>14</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>15</v>
       </c>
       <c r="O15" s="26"/>
-      <c r="P15" s="14">
+      <c r="P15" s="26">
         <v>8</v>
       </c>
       <c r="Q15" s="14"/>
@@ -2449,7 +2455,7 @@
       <c r="O16" s="26">
         <v>2</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="26">
         <v>2</v>
       </c>
       <c r="Q16" s="14">
@@ -2526,7 +2532,7 @@
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
-      <c r="P17" s="14"/>
+      <c r="P17" s="26"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
@@ -2573,7 +2579,7 @@
         <v>7</v>
       </c>
       <c r="O18" s="26"/>
-      <c r="P18" s="14"/>
+      <c r="P18" s="26"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="14"/>
@@ -2626,7 +2632,7 @@
       <c r="O19" s="26">
         <v>12</v>
       </c>
-      <c r="P19" s="14"/>
+      <c r="P19" s="26"/>
       <c r="Q19" s="14">
         <v>12</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>11</v>
       </c>
       <c r="O20" s="26"/>
-      <c r="P20" s="14">
+      <c r="P20" s="26">
         <v>6</v>
       </c>
       <c r="Q20" s="14"/>
@@ -2726,7 +2732,7 @@
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
-      <c r="P21" s="14"/>
+      <c r="P21" s="26"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
       <c r="S21" s="14"/>
@@ -2767,7 +2773,7 @@
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
       <c r="O22" s="26"/>
-      <c r="P22" s="14"/>
+      <c r="P22" s="26"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14"/>
       <c r="S22" s="14"/>
@@ -2816,7 +2822,7 @@
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
-      <c r="P23" s="14"/>
+      <c r="P23" s="26"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
       <c r="S23" s="14"/>
@@ -2859,7 +2865,7 @@
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="14"/>
+      <c r="P24" s="26"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
       <c r="S24" s="14"/>
@@ -2906,8 +2912,8 @@
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
@@ -2951,8 +2957,8 @@
       <c r="L27" s="27"/>
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
       <c r="S27" s="14"/>
@@ -2994,8 +3000,8 @@
       <c r="L28" s="27"/>
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
@@ -3037,8 +3043,8 @@
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
@@ -3080,8 +3086,8 @@
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
       <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
@@ -3123,8 +3129,8 @@
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
       <c r="N31" s="27"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
@@ -3172,8 +3178,8 @@
       <c r="L33" s="27"/>
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
       <c r="S33" s="14"/>
@@ -3219,8 +3225,8 @@
       <c r="L34" s="27"/>
       <c r="M34" s="27"/>
       <c r="N34" s="27"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
       <c r="S34" s="14"/>
@@ -3262,8 +3268,8 @@
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
       <c r="N35" s="27"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
@@ -3305,8 +3311,8 @@
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
       <c r="Q36" s="14"/>
       <c r="R36" s="14"/>
       <c r="S36" s="14"/>
@@ -3348,8 +3354,8 @@
       <c r="L37" s="27"/>
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
       <c r="Q37" s="14"/>
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
@@ -3391,8 +3397,8 @@
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
       <c r="Q38" s="14"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
@@ -3457,7 +3463,7 @@
       <c r="O40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P40" s="14" t="s">
+      <c r="P40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q40" s="14" t="s">
@@ -3556,7 +3562,7 @@
       <c r="O41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P41" s="14" t="s">
+      <c r="P41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q41" s="14" t="s">
@@ -3647,7 +3653,7 @@
       <c r="O42" s="26">
         <v>1</v>
       </c>
-      <c r="P42" s="14">
+      <c r="P42" s="26">
         <v>1</v>
       </c>
       <c r="Q42" s="14">
@@ -3720,7 +3726,7 @@
       <c r="M43" s="26"/>
       <c r="N43" s="26"/>
       <c r="O43" s="26"/>
-      <c r="P43" s="14"/>
+      <c r="P43" s="26"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
       <c r="S43" s="14"/>
@@ -3761,7 +3767,7 @@
       <c r="M44" s="26"/>
       <c r="N44" s="26"/>
       <c r="O44" s="26"/>
-      <c r="P44" s="14"/>
+      <c r="P44" s="26"/>
       <c r="Q44" s="14"/>
       <c r="R44" s="14"/>
       <c r="S44" s="14"/>
@@ -3802,7 +3808,7 @@
       <c r="M45" s="26"/>
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
-      <c r="P45" s="14"/>
+      <c r="P45" s="26"/>
       <c r="Q45" s="14"/>
       <c r="R45" s="14"/>
       <c r="S45" s="14"/>
@@ -3852,8 +3858,8 @@
       <c r="L47" s="27"/>
       <c r="M47" s="27"/>
       <c r="N47" s="27"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
+      <c r="O47" s="27"/>
+      <c r="P47" s="27"/>
       <c r="Q47" s="14"/>
       <c r="R47" s="14"/>
       <c r="S47" s="14"/>
@@ -3901,8 +3907,8 @@
       <c r="L48" s="27"/>
       <c r="M48" s="27"/>
       <c r="N48" s="27"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
       <c r="Q48" s="14"/>
       <c r="R48" s="14"/>
       <c r="S48" s="14"/>
@@ -3948,8 +3954,8 @@
       <c r="L49" s="27"/>
       <c r="M49" s="27"/>
       <c r="N49" s="27"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="27"/>
       <c r="Q49" s="14"/>
       <c r="R49" s="14"/>
       <c r="S49" s="14"/>
@@ -3995,8 +4001,8 @@
       <c r="L50" s="27"/>
       <c r="M50" s="27"/>
       <c r="N50" s="27"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
+      <c r="O50" s="27"/>
+      <c r="P50" s="27"/>
       <c r="Q50" s="14"/>
       <c r="R50" s="14"/>
       <c r="S50" s="14"/>
@@ -4042,8 +4048,8 @@
       <c r="L51" s="27"/>
       <c r="M51" s="27"/>
       <c r="N51" s="27"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="27"/>
       <c r="Q51" s="14"/>
       <c r="R51" s="14"/>
       <c r="S51" s="14"/>
@@ -4089,8 +4095,8 @@
       <c r="L52" s="27"/>
       <c r="M52" s="27"/>
       <c r="N52" s="27"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
       <c r="Q52" s="14"/>
       <c r="R52" s="14"/>
       <c r="S52" s="14"/>
@@ -4136,8 +4142,8 @@
       <c r="L53" s="27"/>
       <c r="M53" s="27"/>
       <c r="N53" s="27"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
+      <c r="O53" s="27"/>
+      <c r="P53" s="27"/>
       <c r="Q53" s="14"/>
       <c r="R53" s="14"/>
       <c r="S53" s="14"/>
@@ -4183,8 +4189,8 @@
       <c r="L54" s="27"/>
       <c r="M54" s="27"/>
       <c r="N54" s="27"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
       <c r="Q54" s="14"/>
       <c r="R54" s="14"/>
       <c r="S54" s="14"/>
@@ -4237,7 +4243,7 @@
       <c r="O56" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P56" s="14" t="s">
+      <c r="P56" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q56" s="14" t="s">
@@ -4294,7 +4300,7 @@
       <c r="O57" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="P57" s="14" t="s">
+      <c r="P57" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Q57" s="14" t="s">
@@ -4342,10 +4348,10 @@
       </c>
       <c r="M58" s="26"/>
       <c r="N58" s="26"/>
-      <c r="O58" s="14">
+      <c r="O58" s="26">
         <v>6</v>
       </c>
-      <c r="P58" s="14"/>
+      <c r="P58" s="26"/>
       <c r="Q58" s="14"/>
       <c r="R58" s="14"/>
       <c r="S58" s="14"/>
@@ -4389,10 +4395,10 @@
         <v>7</v>
       </c>
       <c r="N59" s="26"/>
-      <c r="O59" s="14">
+      <c r="O59" s="26">
         <v>7</v>
       </c>
-      <c r="P59" s="14"/>
+      <c r="P59" s="26"/>
       <c r="Q59" s="14"/>
       <c r="R59" s="14"/>
       <c r="S59" s="14"/>
@@ -4433,7 +4439,7 @@
       <c r="M60" s="26"/>
       <c r="N60" s="26"/>
       <c r="O60" s="26"/>
-      <c r="P60" s="14"/>
+      <c r="P60" s="26"/>
       <c r="Q60" s="14">
         <v>6</v>
       </c>
@@ -4476,7 +4482,7 @@
       <c r="M61" s="26"/>
       <c r="N61" s="26"/>
       <c r="O61" s="26"/>
-      <c r="P61" s="14"/>
+      <c r="P61" s="26"/>
       <c r="Q61" s="14">
         <v>10</v>
       </c>
@@ -4519,7 +4525,7 @@
       <c r="M62" s="26"/>
       <c r="N62" s="26"/>
       <c r="O62" s="26"/>
-      <c r="P62" s="14"/>
+      <c r="P62" s="26"/>
       <c r="Q62" s="14">
         <v>9</v>
       </c>
@@ -4562,7 +4568,7 @@
       <c r="M63" s="26"/>
       <c r="N63" s="26"/>
       <c r="O63" s="26"/>
-      <c r="P63" s="14"/>
+      <c r="P63" s="26"/>
       <c r="Q63" s="14">
         <v>7</v>
       </c>
@@ -4605,7 +4611,7 @@
       <c r="M64" s="26"/>
       <c r="N64" s="26"/>
       <c r="O64" s="26"/>
-      <c r="P64" s="14"/>
+      <c r="P64" s="26"/>
       <c r="Q64" s="14">
         <v>8</v>
       </c>
@@ -4650,7 +4656,7 @@
         <v>3</v>
       </c>
       <c r="O65" s="26"/>
-      <c r="P65" s="14"/>
+      <c r="P65" s="26"/>
       <c r="Q65" s="14"/>
       <c r="R65" s="14"/>
       <c r="S65" s="14"/>
@@ -4693,7 +4699,7 @@
       <c r="M66" s="26"/>
       <c r="N66" s="26"/>
       <c r="O66" s="26"/>
-      <c r="P66" s="14"/>
+      <c r="P66" s="26"/>
       <c r="Q66" s="14">
         <v>11</v>
       </c>
@@ -4742,7 +4748,7 @@
       <c r="O67" s="26">
         <v>8</v>
       </c>
-      <c r="P67" s="14"/>
+      <c r="P67" s="26"/>
       <c r="Q67" s="14"/>
       <c r="R67" s="14"/>
       <c r="S67" s="14"/>
@@ -4789,7 +4795,7 @@
       <c r="O68" s="26">
         <v>9</v>
       </c>
-      <c r="P68" s="14"/>
+      <c r="P68" s="26"/>
       <c r="Q68" s="14"/>
       <c r="R68" s="14"/>
       <c r="S68" s="14"/>
@@ -4831,8 +4837,8 @@
       <c r="L70" s="27"/>
       <c r="M70" s="27"/>
       <c r="N70" s="27"/>
-      <c r="O70" s="14"/>
-      <c r="P70" s="14"/>
+      <c r="O70" s="27"/>
+      <c r="P70" s="27"/>
       <c r="Q70" s="14"/>
       <c r="R70" s="14"/>
       <c r="S70" s="14" t="s">
@@ -4902,8 +4908,8 @@
       <c r="L71" s="27"/>
       <c r="M71" s="27"/>
       <c r="N71" s="27"/>
-      <c r="O71" s="14"/>
-      <c r="P71" s="14"/>
+      <c r="O71" s="27"/>
+      <c r="P71" s="27"/>
       <c r="Q71" s="14"/>
       <c r="R71" s="14"/>
       <c r="S71" s="14" t="s">
@@ -4973,8 +4979,8 @@
       <c r="L72" s="27"/>
       <c r="M72" s="27"/>
       <c r="N72" s="27"/>
-      <c r="O72" s="14"/>
-      <c r="P72" s="14"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="27"/>
       <c r="Q72" s="14"/>
       <c r="R72" s="14"/>
       <c r="S72" s="14">
@@ -5038,8 +5044,8 @@
       <c r="L73" s="27"/>
       <c r="M73" s="27"/>
       <c r="N73" s="27"/>
-      <c r="O73" s="14"/>
-      <c r="P73" s="14"/>
+      <c r="O73" s="27"/>
+      <c r="P73" s="27"/>
       <c r="Q73" s="14"/>
       <c r="R73" s="14"/>
       <c r="S73" s="14">
@@ -5107,8 +5113,8 @@
       <c r="L74" s="27"/>
       <c r="M74" s="27"/>
       <c r="N74" s="27"/>
-      <c r="O74" s="14"/>
-      <c r="P74" s="14"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="27"/>
       <c r="Q74" s="14"/>
       <c r="R74" s="14"/>
       <c r="S74" s="14"/>
@@ -5150,8 +5156,8 @@
       <c r="L75" s="27"/>
       <c r="M75" s="27"/>
       <c r="N75" s="27"/>
-      <c r="O75" s="14"/>
-      <c r="P75" s="14"/>
+      <c r="O75" s="27"/>
+      <c r="P75" s="27"/>
       <c r="Q75" s="14"/>
       <c r="R75" s="14"/>
       <c r="S75" s="14"/>
@@ -5197,8 +5203,8 @@
       <c r="L76" s="27"/>
       <c r="M76" s="27"/>
       <c r="N76" s="27"/>
-      <c r="O76" s="14"/>
-      <c r="P76" s="14"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="27"/>
       <c r="Q76" s="14"/>
       <c r="R76" s="14"/>
       <c r="S76" s="14"/>
@@ -5242,8 +5248,8 @@
       <c r="L77" s="27"/>
       <c r="M77" s="27"/>
       <c r="N77" s="27"/>
-      <c r="O77" s="14"/>
-      <c r="P77" s="14"/>
+      <c r="O77" s="27"/>
+      <c r="P77" s="27"/>
       <c r="Q77" s="14"/>
       <c r="R77" s="14"/>
       <c r="S77" s="14"/>
@@ -5287,8 +5293,8 @@
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
       <c r="N78" s="27"/>
-      <c r="O78" s="14"/>
-      <c r="P78" s="14"/>
+      <c r="O78" s="27"/>
+      <c r="P78" s="27"/>
       <c r="Q78" s="14"/>
       <c r="R78" s="14"/>
       <c r="S78" s="14"/>
@@ -5330,8 +5336,8 @@
       <c r="L79" s="27"/>
       <c r="M79" s="27"/>
       <c r="N79" s="27"/>
-      <c r="O79" s="14"/>
-      <c r="P79" s="14"/>
+      <c r="O79" s="27"/>
+      <c r="P79" s="27"/>
       <c r="Q79" s="14"/>
       <c r="R79" s="14"/>
       <c r="S79" s="14"/>
@@ -5373,8 +5379,8 @@
       <c r="L80" s="27"/>
       <c r="M80" s="27"/>
       <c r="N80" s="27"/>
-      <c r="O80" s="14"/>
-      <c r="P80" s="14"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="27"/>
       <c r="Q80" s="14"/>
       <c r="R80" s="14"/>
       <c r="S80" s="14">
@@ -5416,8 +5422,8 @@
       <c r="L81" s="27"/>
       <c r="M81" s="27"/>
       <c r="N81" s="27"/>
-      <c r="O81" s="14"/>
-      <c r="P81" s="14"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="27"/>
       <c r="Q81" s="14"/>
       <c r="R81" s="14"/>
       <c r="S81" s="14">
@@ -5465,8 +5471,8 @@
       <c r="L83" s="27"/>
       <c r="M83" s="27"/>
       <c r="N83" s="27"/>
-      <c r="O83" s="14"/>
-      <c r="P83" s="14"/>
+      <c r="O83" s="27"/>
+      <c r="P83" s="27"/>
       <c r="Q83" s="14"/>
       <c r="R83" s="14"/>
       <c r="S83" s="14"/>
@@ -5510,8 +5516,8 @@
       <c r="L84" s="27"/>
       <c r="M84" s="27"/>
       <c r="N84" s="27"/>
-      <c r="O84" s="14"/>
-      <c r="P84" s="14"/>
+      <c r="O84" s="27"/>
+      <c r="P84" s="27"/>
       <c r="Q84" s="14"/>
       <c r="R84" s="14"/>
       <c r="S84" s="14"/>
@@ -5551,8 +5557,8 @@
       <c r="L85" s="27"/>
       <c r="M85" s="27"/>
       <c r="N85" s="27"/>
-      <c r="O85" s="14"/>
-      <c r="P85" s="14"/>
+      <c r="O85" s="27"/>
+      <c r="P85" s="27"/>
       <c r="Q85" s="14"/>
       <c r="R85" s="14"/>
       <c r="S85" s="14"/>
@@ -5592,8 +5598,8 @@
       <c r="L86" s="27"/>
       <c r="M86" s="27"/>
       <c r="N86" s="27"/>
-      <c r="O86" s="14"/>
-      <c r="P86" s="14"/>
+      <c r="O86" s="27"/>
+      <c r="P86" s="27"/>
       <c r="Q86" s="14"/>
       <c r="R86" s="14"/>
       <c r="S86" s="14"/>
@@ -5633,8 +5639,8 @@
       <c r="L87" s="27"/>
       <c r="M87" s="27"/>
       <c r="N87" s="27"/>
-      <c r="O87" s="14"/>
-      <c r="P87" s="14"/>
+      <c r="O87" s="27"/>
+      <c r="P87" s="27"/>
       <c r="Q87" s="14"/>
       <c r="R87" s="14"/>
       <c r="S87" s="14"/>
@@ -5675,10 +5681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6088,6 +6094,20 @@
         <v>177</v>
       </c>
       <c r="D28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Other bibliographical production were added.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5DC29-A778-4D85-AF74-77B051367D21}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="200">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -602,6 +603,30 @@
   </si>
   <si>
     <t>Traducciones</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otra producción bibliográfica - Prólogo</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otra producción bibliográfica - Introducción</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otra producción bibliográfica - Epílogo</t>
+  </si>
+  <si>
+    <t>Producción bibliográfica - Otra producción bibliográfica - Otra</t>
+  </si>
+  <si>
+    <t>Introducción</t>
+  </si>
+  <si>
+    <t>Prólogo</t>
+  </si>
+  <si>
+    <t>Epílogo</t>
+  </si>
+  <si>
+    <t>Otra</t>
   </si>
 </sst>
 </file>
@@ -863,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -973,6 +998,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1319,10 +1347,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="T83" sqref="T83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1555,7 @@
       <c r="Q3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S3" s="14" t="s">
@@ -1624,7 +1652,7 @@
       <c r="Q4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S4" s="14" t="s">
@@ -1721,7 +1749,7 @@
       <c r="Q5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S5" s="14" t="s">
@@ -1814,7 +1842,7 @@
       <c r="Q6" s="26">
         <v>3</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="26">
         <v>3</v>
       </c>
       <c r="S6" s="14">
@@ -1891,7 +1919,7 @@
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
-      <c r="R7" s="14"/>
+      <c r="R7" s="26"/>
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
       <c r="U7" s="14"/>
@@ -1934,7 +1962,7 @@
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
-      <c r="R8" s="14"/>
+      <c r="R8" s="26"/>
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
@@ -1979,7 +2007,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
-      <c r="R9" s="14"/>
+      <c r="R9" s="26"/>
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
@@ -2036,7 +2064,7 @@
       <c r="Q10" s="26">
         <v>4</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="26">
         <v>4</v>
       </c>
       <c r="S10" s="14">
@@ -2123,7 +2151,7 @@
       <c r="Q11" s="26">
         <v>5</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="26">
         <v>5</v>
       </c>
       <c r="S11" s="14">
@@ -2198,7 +2226,7 @@
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
-      <c r="R12" s="14"/>
+      <c r="R12" s="26"/>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
@@ -2249,7 +2277,7 @@
       <c r="Q13" s="26">
         <v>13</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="26">
         <v>7</v>
       </c>
       <c r="S13" s="14">
@@ -2326,7 +2354,7 @@
       <c r="Q14" s="26">
         <v>14</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14" s="26">
         <v>8</v>
       </c>
       <c r="S14" s="14">
@@ -2401,7 +2429,7 @@
         <v>8</v>
       </c>
       <c r="Q15" s="26"/>
-      <c r="R15" s="14"/>
+      <c r="R15" s="26"/>
       <c r="S15" s="14">
         <v>12</v>
       </c>
@@ -2482,7 +2510,7 @@
       <c r="Q16" s="26">
         <v>2</v>
       </c>
-      <c r="R16" s="14">
+      <c r="R16" s="26">
         <v>2</v>
       </c>
       <c r="S16" s="14">
@@ -2555,7 +2583,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
-      <c r="R17" s="14"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
@@ -2602,7 +2630,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
-      <c r="R18" s="14"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="14"/>
       <c r="T18" s="14"/>
       <c r="U18" s="14"/>
@@ -2657,7 +2685,7 @@
       <c r="Q19" s="26">
         <v>12</v>
       </c>
-      <c r="R19" s="14"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
@@ -2704,7 +2732,7 @@
         <v>6</v>
       </c>
       <c r="Q20" s="26"/>
-      <c r="R20" s="14">
+      <c r="R20" s="26">
         <v>6</v>
       </c>
       <c r="S20" s="14"/>
@@ -2755,7 +2783,7 @@
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
-      <c r="R21" s="14"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
       <c r="U21" s="14"/>
@@ -2796,7 +2824,7 @@
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
-      <c r="R22" s="14"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
       <c r="U22" s="14"/>
@@ -2845,7 +2873,7 @@
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
-      <c r="R23" s="14"/>
+      <c r="R23" s="26"/>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
       <c r="U23" s="14"/>
@@ -2888,7 +2916,7 @@
       <c r="O24" s="26"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
-      <c r="R24" s="14"/>
+      <c r="R24" s="26"/>
       <c r="S24" s="14"/>
       <c r="T24" s="14"/>
       <c r="U24" s="14"/>
@@ -2936,7 +2964,7 @@
       <c r="O26" s="27"/>
       <c r="P26" s="27"/>
       <c r="Q26" s="27"/>
-      <c r="R26" s="14"/>
+      <c r="R26" s="27"/>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
       <c r="U26" s="14"/>
@@ -2981,7 +3009,7 @@
       <c r="O27" s="27"/>
       <c r="P27" s="27"/>
       <c r="Q27" s="27"/>
-      <c r="R27" s="14"/>
+      <c r="R27" s="27"/>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
       <c r="U27" s="14"/>
@@ -3024,7 +3052,7 @@
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
-      <c r="R28" s="14"/>
+      <c r="R28" s="27"/>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
       <c r="U28" s="14"/>
@@ -3067,7 +3095,7 @@
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
       <c r="Q29" s="27"/>
-      <c r="R29" s="14"/>
+      <c r="R29" s="27"/>
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
       <c r="U29" s="14"/>
@@ -3110,7 +3138,7 @@
       <c r="O30" s="27"/>
       <c r="P30" s="27"/>
       <c r="Q30" s="27"/>
-      <c r="R30" s="14"/>
+      <c r="R30" s="27"/>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
@@ -3153,7 +3181,7 @@
       <c r="O31" s="27"/>
       <c r="P31" s="27"/>
       <c r="Q31" s="27"/>
-      <c r="R31" s="14"/>
+      <c r="R31" s="27"/>
       <c r="S31" s="14"/>
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
@@ -3202,7 +3230,7 @@
       <c r="O33" s="27"/>
       <c r="P33" s="27"/>
       <c r="Q33" s="27"/>
-      <c r="R33" s="14"/>
+      <c r="R33" s="27"/>
       <c r="S33" s="14"/>
       <c r="T33" s="14"/>
       <c r="U33" s="14"/>
@@ -3249,7 +3277,7 @@
       <c r="O34" s="27"/>
       <c r="P34" s="27"/>
       <c r="Q34" s="27"/>
-      <c r="R34" s="14"/>
+      <c r="R34" s="27"/>
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
       <c r="U34" s="14"/>
@@ -3292,7 +3320,7 @@
       <c r="O35" s="27"/>
       <c r="P35" s="27"/>
       <c r="Q35" s="27"/>
-      <c r="R35" s="14"/>
+      <c r="R35" s="27"/>
       <c r="S35" s="14"/>
       <c r="T35" s="14"/>
       <c r="U35" s="14"/>
@@ -3335,7 +3363,7 @@
       <c r="O36" s="27"/>
       <c r="P36" s="27"/>
       <c r="Q36" s="27"/>
-      <c r="R36" s="14"/>
+      <c r="R36" s="27"/>
       <c r="S36" s="14"/>
       <c r="T36" s="14"/>
       <c r="U36" s="14"/>
@@ -3378,7 +3406,7 @@
       <c r="O37" s="27"/>
       <c r="P37" s="27"/>
       <c r="Q37" s="27"/>
-      <c r="R37" s="14"/>
+      <c r="R37" s="27"/>
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
       <c r="U37" s="14"/>
@@ -3421,7 +3449,7 @@
       <c r="O38" s="27"/>
       <c r="P38" s="27"/>
       <c r="Q38" s="27"/>
-      <c r="R38" s="14"/>
+      <c r="R38" s="27"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
       <c r="U38" s="14"/>
@@ -3490,7 +3518,7 @@
       <c r="Q40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R40" s="14" t="s">
+      <c r="R40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S40" s="14" t="s">
@@ -3589,7 +3617,7 @@
       <c r="Q41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R41" s="14" t="s">
+      <c r="R41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S41" s="14" t="s">
@@ -3680,7 +3708,7 @@
       <c r="Q42" s="26">
         <v>1</v>
       </c>
-      <c r="R42" s="14">
+      <c r="R42" s="26">
         <v>1</v>
       </c>
       <c r="S42" s="14">
@@ -3749,7 +3777,7 @@
       <c r="O43" s="26"/>
       <c r="P43" s="26"/>
       <c r="Q43" s="26"/>
-      <c r="R43" s="14"/>
+      <c r="R43" s="26"/>
       <c r="S43" s="14"/>
       <c r="T43" s="14"/>
       <c r="U43" s="14"/>
@@ -3790,7 +3818,7 @@
       <c r="O44" s="26"/>
       <c r="P44" s="26"/>
       <c r="Q44" s="26"/>
-      <c r="R44" s="14"/>
+      <c r="R44" s="26"/>
       <c r="S44" s="14"/>
       <c r="T44" s="14"/>
       <c r="U44" s="14"/>
@@ -3831,7 +3859,7 @@
       <c r="O45" s="26"/>
       <c r="P45" s="26"/>
       <c r="Q45" s="26"/>
-      <c r="R45" s="14"/>
+      <c r="R45" s="26"/>
       <c r="S45" s="14"/>
       <c r="T45" s="14"/>
       <c r="U45" s="14"/>
@@ -3882,7 +3910,7 @@
       <c r="O47" s="27"/>
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
-      <c r="R47" s="14"/>
+      <c r="R47" s="27"/>
       <c r="S47" s="14"/>
       <c r="T47" s="14"/>
       <c r="U47" s="14"/>
@@ -3931,7 +3959,7 @@
       <c r="O48" s="27"/>
       <c r="P48" s="27"/>
       <c r="Q48" s="27"/>
-      <c r="R48" s="14"/>
+      <c r="R48" s="27"/>
       <c r="S48" s="14"/>
       <c r="T48" s="14"/>
       <c r="U48" s="14"/>
@@ -3978,7 +4006,7 @@
       <c r="O49" s="27"/>
       <c r="P49" s="27"/>
       <c r="Q49" s="27"/>
-      <c r="R49" s="14"/>
+      <c r="R49" s="27"/>
       <c r="S49" s="14"/>
       <c r="T49" s="14"/>
       <c r="U49" s="14"/>
@@ -4025,7 +4053,7 @@
       <c r="O50" s="27"/>
       <c r="P50" s="27"/>
       <c r="Q50" s="27"/>
-      <c r="R50" s="14"/>
+      <c r="R50" s="27"/>
       <c r="S50" s="14"/>
       <c r="T50" s="14"/>
       <c r="U50" s="14"/>
@@ -4072,7 +4100,7 @@
       <c r="O51" s="27"/>
       <c r="P51" s="27"/>
       <c r="Q51" s="27"/>
-      <c r="R51" s="14"/>
+      <c r="R51" s="27"/>
       <c r="S51" s="14"/>
       <c r="T51" s="14"/>
       <c r="U51" s="14"/>
@@ -4119,7 +4147,7 @@
       <c r="O52" s="27"/>
       <c r="P52" s="27"/>
       <c r="Q52" s="27"/>
-      <c r="R52" s="14"/>
+      <c r="R52" s="27"/>
       <c r="S52" s="14"/>
       <c r="T52" s="14"/>
       <c r="U52" s="14"/>
@@ -4166,7 +4194,7 @@
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
       <c r="Q53" s="27"/>
-      <c r="R53" s="14"/>
+      <c r="R53" s="27"/>
       <c r="S53" s="14"/>
       <c r="T53" s="14"/>
       <c r="U53" s="14"/>
@@ -4213,7 +4241,7 @@
       <c r="O54" s="27"/>
       <c r="P54" s="27"/>
       <c r="Q54" s="27"/>
-      <c r="R54" s="14"/>
+      <c r="R54" s="27"/>
       <c r="S54" s="14"/>
       <c r="T54" s="14"/>
       <c r="U54" s="14"/>
@@ -4270,7 +4298,7 @@
       <c r="Q56" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R56" s="14" t="s">
+      <c r="R56" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S56" s="14"/>
@@ -4327,7 +4355,7 @@
       <c r="Q57" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="R57" s="14" t="s">
+      <c r="R57" s="26" t="s">
         <v>55</v>
       </c>
       <c r="S57" s="14"/>
@@ -4374,7 +4402,7 @@
       </c>
       <c r="P58" s="26"/>
       <c r="Q58" s="26"/>
-      <c r="R58" s="14"/>
+      <c r="R58" s="26"/>
       <c r="S58" s="14"/>
       <c r="T58" s="14"/>
       <c r="U58" s="14"/>
@@ -4421,7 +4449,7 @@
       </c>
       <c r="P59" s="26"/>
       <c r="Q59" s="26"/>
-      <c r="R59" s="14"/>
+      <c r="R59" s="26"/>
       <c r="S59" s="14"/>
       <c r="T59" s="14"/>
       <c r="U59" s="14"/>
@@ -4464,7 +4492,7 @@
       <c r="Q60" s="26">
         <v>6</v>
       </c>
-      <c r="R60" s="14"/>
+      <c r="R60" s="26"/>
       <c r="S60" s="14"/>
       <c r="T60" s="14"/>
       <c r="U60" s="14"/>
@@ -4507,7 +4535,7 @@
       <c r="Q61" s="26">
         <v>10</v>
       </c>
-      <c r="R61" s="14"/>
+      <c r="R61" s="26"/>
       <c r="S61" s="14"/>
       <c r="T61" s="14"/>
       <c r="U61" s="14"/>
@@ -4550,7 +4578,7 @@
       <c r="Q62" s="26">
         <v>9</v>
       </c>
-      <c r="R62" s="14"/>
+      <c r="R62" s="26"/>
       <c r="S62" s="14"/>
       <c r="T62" s="14"/>
       <c r="U62" s="14"/>
@@ -4593,7 +4621,7 @@
       <c r="Q63" s="26">
         <v>7</v>
       </c>
-      <c r="R63" s="14"/>
+      <c r="R63" s="26"/>
       <c r="S63" s="14"/>
       <c r="T63" s="14"/>
       <c r="U63" s="14"/>
@@ -4636,7 +4664,7 @@
       <c r="Q64" s="26">
         <v>8</v>
       </c>
-      <c r="R64" s="14"/>
+      <c r="R64" s="26"/>
       <c r="S64" s="14"/>
       <c r="T64" s="14"/>
       <c r="U64" s="14"/>
@@ -4679,7 +4707,7 @@
       <c r="O65" s="26"/>
       <c r="P65" s="26"/>
       <c r="Q65" s="26"/>
-      <c r="R65" s="14"/>
+      <c r="R65" s="26"/>
       <c r="S65" s="14"/>
       <c r="T65" s="14"/>
       <c r="U65" s="14"/>
@@ -4724,7 +4752,7 @@
       <c r="Q66" s="26">
         <v>11</v>
       </c>
-      <c r="R66" s="14"/>
+      <c r="R66" s="26"/>
       <c r="S66" s="14"/>
       <c r="T66" s="14"/>
       <c r="U66" s="14"/>
@@ -4771,7 +4799,7 @@
       </c>
       <c r="P67" s="26"/>
       <c r="Q67" s="26"/>
-      <c r="R67" s="14"/>
+      <c r="R67" s="26"/>
       <c r="S67" s="14"/>
       <c r="T67" s="14"/>
       <c r="U67" s="14"/>
@@ -4818,7 +4846,7 @@
       </c>
       <c r="P68" s="26"/>
       <c r="Q68" s="26"/>
-      <c r="R68" s="14"/>
+      <c r="R68" s="26"/>
       <c r="S68" s="14"/>
       <c r="T68" s="14"/>
       <c r="U68" s="14"/>
@@ -4861,7 +4889,7 @@
       <c r="O70" s="27"/>
       <c r="P70" s="27"/>
       <c r="Q70" s="27"/>
-      <c r="R70" s="14"/>
+      <c r="R70" s="27"/>
       <c r="S70" s="14" t="s">
         <v>55</v>
       </c>
@@ -4932,7 +4960,7 @@
       <c r="O71" s="27"/>
       <c r="P71" s="27"/>
       <c r="Q71" s="27"/>
-      <c r="R71" s="14"/>
+      <c r="R71" s="27"/>
       <c r="S71" s="14" t="s">
         <v>55</v>
       </c>
@@ -5003,7 +5031,7 @@
       <c r="O72" s="27"/>
       <c r="P72" s="27"/>
       <c r="Q72" s="27"/>
-      <c r="R72" s="14"/>
+      <c r="R72" s="27"/>
       <c r="S72" s="14">
         <v>4</v>
       </c>
@@ -5068,7 +5096,7 @@
       <c r="O73" s="27"/>
       <c r="P73" s="27"/>
       <c r="Q73" s="27"/>
-      <c r="R73" s="14"/>
+      <c r="R73" s="27"/>
       <c r="S73" s="14">
         <v>5</v>
       </c>
@@ -5137,7 +5165,7 @@
       <c r="O74" s="27"/>
       <c r="P74" s="27"/>
       <c r="Q74" s="27"/>
-      <c r="R74" s="14"/>
+      <c r="R74" s="27"/>
       <c r="S74" s="14"/>
       <c r="T74" s="14"/>
       <c r="U74" s="14"/>
@@ -5180,7 +5208,7 @@
       <c r="O75" s="27"/>
       <c r="P75" s="27"/>
       <c r="Q75" s="27"/>
-      <c r="R75" s="14"/>
+      <c r="R75" s="27"/>
       <c r="S75" s="14"/>
       <c r="T75" s="14"/>
       <c r="U75" s="14"/>
@@ -5227,7 +5255,7 @@
       <c r="O76" s="27"/>
       <c r="P76" s="27"/>
       <c r="Q76" s="27"/>
-      <c r="R76" s="14"/>
+      <c r="R76" s="27"/>
       <c r="S76" s="14"/>
       <c r="T76" s="14"/>
       <c r="U76" s="14"/>
@@ -5272,7 +5300,7 @@
       <c r="O77" s="27"/>
       <c r="P77" s="27"/>
       <c r="Q77" s="27"/>
-      <c r="R77" s="14"/>
+      <c r="R77" s="27"/>
       <c r="S77" s="14"/>
       <c r="T77" s="14"/>
       <c r="U77" s="14"/>
@@ -5317,7 +5345,7 @@
       <c r="O78" s="27"/>
       <c r="P78" s="27"/>
       <c r="Q78" s="27"/>
-      <c r="R78" s="14"/>
+      <c r="R78" s="27"/>
       <c r="S78" s="14"/>
       <c r="T78" s="14"/>
       <c r="U78" s="14"/>
@@ -5360,7 +5388,7 @@
       <c r="O79" s="27"/>
       <c r="P79" s="27"/>
       <c r="Q79" s="27"/>
-      <c r="R79" s="14"/>
+      <c r="R79" s="27"/>
       <c r="S79" s="14"/>
       <c r="T79" s="14"/>
       <c r="U79" s="14"/>
@@ -5403,7 +5431,7 @@
       <c r="O80" s="27"/>
       <c r="P80" s="27"/>
       <c r="Q80" s="27"/>
-      <c r="R80" s="14"/>
+      <c r="R80" s="27"/>
       <c r="S80" s="14">
         <v>8</v>
       </c>
@@ -5446,7 +5474,7 @@
       <c r="O81" s="27"/>
       <c r="P81" s="27"/>
       <c r="Q81" s="27"/>
-      <c r="R81" s="14"/>
+      <c r="R81" s="27"/>
       <c r="S81" s="14">
         <v>9</v>
       </c>
@@ -5495,7 +5523,7 @@
       <c r="O83" s="27"/>
       <c r="P83" s="27"/>
       <c r="Q83" s="27"/>
-      <c r="R83" s="14"/>
+      <c r="R83" s="27"/>
       <c r="S83" s="14"/>
       <c r="T83" s="14"/>
       <c r="U83" s="14"/>
@@ -5540,7 +5568,7 @@
       <c r="O84" s="27"/>
       <c r="P84" s="27"/>
       <c r="Q84" s="27"/>
-      <c r="R84" s="14"/>
+      <c r="R84" s="27"/>
       <c r="S84" s="14"/>
       <c r="T84" s="14"/>
       <c r="U84" s="14"/>
@@ -5581,7 +5609,7 @@
       <c r="O85" s="27"/>
       <c r="P85" s="27"/>
       <c r="Q85" s="27"/>
-      <c r="R85" s="14"/>
+      <c r="R85" s="27"/>
       <c r="S85" s="14"/>
       <c r="T85" s="14"/>
       <c r="U85" s="14"/>
@@ -5622,7 +5650,7 @@
       <c r="O86" s="27"/>
       <c r="P86" s="27"/>
       <c r="Q86" s="27"/>
-      <c r="R86" s="14"/>
+      <c r="R86" s="27"/>
       <c r="S86" s="14"/>
       <c r="T86" s="14"/>
       <c r="U86" s="14"/>
@@ -5663,7 +5691,7 @@
       <c r="O87" s="27"/>
       <c r="P87" s="27"/>
       <c r="Q87" s="27"/>
-      <c r="R87" s="14"/>
+      <c r="R87" s="27"/>
       <c r="S87" s="14"/>
       <c r="T87" s="14"/>
       <c r="U87" s="14"/>
@@ -5702,10 +5730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6172,6 +6200,62 @@
       </c>
       <c r="D32" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="C36" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Technical Production was added
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F28D20-40BB-4110-B70B-093B72BA0238}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94153D06-343E-46D5-A477-5C37E2B1ED91}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="211">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -633,6 +633,33 @@
   </si>
   <si>
     <t>Software</t>
+  </si>
+  <si>
+    <t>Producción técnica - Productos tecnológicos - Gen Clonado</t>
+  </si>
+  <si>
+    <t>Producción técnica - Productos tecnológicos - Coleccion biologica de referencia con informacion sistematizada</t>
+  </si>
+  <si>
+    <t>Producción técnica - Productos tecnológicos - Otro</t>
+  </si>
+  <si>
+    <t>Productos tecnológicos - Gen Clonado</t>
+  </si>
+  <si>
+    <t>Productos tecnológicos - Coleccion biologica de referencia con informacion sistematizada</t>
+  </si>
+  <si>
+    <t>Productos tecnológicos - Otro</t>
+  </si>
+  <si>
+    <t>Base de datos de referencia para investigacion</t>
+  </si>
+  <si>
+    <t>Productos Tecnológicos</t>
+  </si>
+  <si>
+    <t>Producción técnica - Productos tecnológicos - Base de datos de referencia para investigación</t>
   </si>
 </sst>
 </file>
@@ -984,6 +1011,15 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -991,6 +1027,12 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1001,21 +1043,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,10 +1389,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="K40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S81" sqref="S74:S81"/>
+      <selection pane="bottomRight" activeCell="AB15" sqref="AB15:AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,40 +1413,40 @@
       <c r="F1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="35" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36" t="s">
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="31" t="s">
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
       <c r="AG1" s="6" t="s">
         <v>32</v>
       </c>
@@ -1519,7 +1546,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="35" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -1576,7 +1603,7 @@
       <c r="S3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U3" s="14" t="s">
@@ -1620,7 +1647,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="17" t="s">
         <v>96</v>
       </c>
@@ -1673,7 +1700,7 @@
       <c r="S4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U4" s="14" t="s">
@@ -1717,7 +1744,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="17" t="s">
         <v>96</v>
       </c>
@@ -1770,7 +1797,7 @@
       <c r="S5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U5" s="14" t="s">
@@ -1814,7 +1841,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
         <v>79</v>
@@ -1863,7 +1890,7 @@
       <c r="S6" s="26">
         <v>3</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6" s="26">
         <v>3</v>
       </c>
       <c r="U6" s="14">
@@ -1907,7 +1934,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="25" t="s">
         <v>96</v>
       </c>
@@ -1936,7 +1963,7 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
-      <c r="T7" s="14"/>
+      <c r="T7" s="26"/>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
@@ -1952,7 +1979,7 @@
       <c r="AG7" s="14"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
         <v>79</v>
@@ -1979,7 +2006,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="26"/>
       <c r="S8" s="26"/>
-      <c r="T8" s="14"/>
+      <c r="T8" s="26"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
@@ -1995,7 +2022,7 @@
       <c r="AG8" s="14"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
         <v>79</v>
@@ -2024,7 +2051,7 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
       <c r="S9" s="26"/>
-      <c r="T9" s="14"/>
+      <c r="T9" s="26"/>
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
       <c r="W9" s="14"/>
@@ -2040,7 +2067,7 @@
       <c r="AG9" s="14"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
         <v>79</v>
@@ -2085,7 +2112,7 @@
       <c r="S10" s="26">
         <v>6</v>
       </c>
-      <c r="T10" s="14">
+      <c r="T10" s="26">
         <v>6</v>
       </c>
       <c r="U10" s="14">
@@ -2127,7 +2154,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="17"/>
       <c r="C11" s="19" t="s">
         <v>77</v>
@@ -2172,7 +2199,7 @@
       <c r="S11" s="26">
         <v>7</v>
       </c>
-      <c r="T11" s="14">
+      <c r="T11" s="26">
         <v>7</v>
       </c>
       <c r="U11" s="14">
@@ -2216,7 +2243,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
         <v>79</v>
@@ -2243,7 +2270,7 @@
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
       <c r="S12" s="26"/>
-      <c r="T12" s="14"/>
+      <c r="T12" s="26"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
       <c r="W12" s="14"/>
@@ -2259,7 +2286,7 @@
       <c r="AG12" s="14"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
         <v>79</v>
@@ -2298,7 +2325,7 @@
       <c r="S13" s="26">
         <v>10</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="26">
         <v>8</v>
       </c>
       <c r="U13" s="14">
@@ -2338,7 +2365,7 @@
       <c r="AG13" s="14"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="17"/>
       <c r="C14" s="19" t="s">
         <v>79</v>
@@ -2375,7 +2402,7 @@
       <c r="S14" s="26">
         <v>11</v>
       </c>
-      <c r="T14" s="14">
+      <c r="T14" s="26">
         <v>9</v>
       </c>
       <c r="U14" s="14">
@@ -2415,7 +2442,7 @@
       <c r="AG14" s="14"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
         <v>79</v>
@@ -2448,7 +2475,7 @@
       <c r="S15" s="26">
         <v>12</v>
       </c>
-      <c r="T15" s="14">
+      <c r="T15" s="26">
         <v>10</v>
       </c>
       <c r="U15" s="14">
@@ -2488,7 +2515,7 @@
       <c r="AG15" s="14"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
         <v>79</v>
@@ -2531,7 +2558,7 @@
       <c r="S16" s="26">
         <v>2</v>
       </c>
-      <c r="T16" s="14">
+      <c r="T16" s="26">
         <v>2</v>
       </c>
       <c r="U16" s="14">
@@ -2573,7 +2600,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
         <v>79</v>
@@ -2600,7 +2627,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
-      <c r="T17" s="14"/>
+      <c r="T17" s="26"/>
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
@@ -2616,7 +2643,7 @@
       <c r="AG17" s="14"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
         <v>79</v>
@@ -2647,7 +2674,7 @@
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
-      <c r="T18" s="14"/>
+      <c r="T18" s="26"/>
       <c r="U18" s="14"/>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
@@ -2667,7 +2694,7 @@
       <c r="AG18" s="14"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="17"/>
       <c r="C19" s="19" t="s">
         <v>79</v>
@@ -2702,7 +2729,7 @@
       </c>
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
-      <c r="T19" s="14"/>
+      <c r="T19" s="26"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
@@ -2718,7 +2745,7 @@
       <c r="AG19" s="14"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="17"/>
       <c r="C20" s="19" t="s">
         <v>79</v>
@@ -2751,7 +2778,7 @@
         <v>6</v>
       </c>
       <c r="S20" s="26"/>
-      <c r="T20" s="14"/>
+      <c r="T20" s="26"/>
       <c r="U20" s="14"/>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
@@ -2773,7 +2800,7 @@
       <c r="AG20" s="14"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="17"/>
       <c r="C21" s="19" t="s">
         <v>79</v>
@@ -2800,7 +2827,7 @@
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
-      <c r="T21" s="14"/>
+      <c r="T21" s="26"/>
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
       <c r="W21" s="14"/>
@@ -2816,7 +2843,7 @@
       <c r="AG21" s="14"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="17"/>
       <c r="C22" s="19" t="s">
         <v>79</v>
@@ -2841,7 +2868,7 @@
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
-      <c r="T22" s="14"/>
+      <c r="T22" s="26"/>
       <c r="U22" s="14"/>
       <c r="V22" s="14"/>
       <c r="W22" s="14"/>
@@ -2859,7 +2886,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="17"/>
       <c r="C23" s="19" t="s">
         <v>79</v>
@@ -2890,7 +2917,7 @@
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
       <c r="S23" s="26"/>
-      <c r="T23" s="14"/>
+      <c r="T23" s="26"/>
       <c r="U23" s="14"/>
       <c r="V23" s="14"/>
       <c r="W23" s="14"/>
@@ -2906,7 +2933,7 @@
       <c r="AG23" s="14"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="17"/>
       <c r="C24" s="19" t="s">
         <v>79</v>
@@ -2933,7 +2960,7 @@
       <c r="Q24" s="26"/>
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
-      <c r="T24" s="14"/>
+      <c r="T24" s="26"/>
       <c r="U24" s="14"/>
       <c r="V24" s="14"/>
       <c r="W24" s="14"/>
@@ -2950,7 +2977,7 @@
     </row>
     <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:33" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="37" t="s">
         <v>53</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -2997,7 +3024,7 @@
       <c r="AG26" s="27"/>
     </row>
     <row r="27" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="17" t="s">
         <v>96</v>
       </c>
@@ -3042,7 +3069,7 @@
       <c r="AG27" s="27"/>
     </row>
     <row r="28" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="12"/>
       <c r="C28" s="19" t="s">
         <v>79</v>
@@ -3085,7 +3112,7 @@
       <c r="AG28" s="27"/>
     </row>
     <row r="29" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="12"/>
       <c r="C29" s="19" t="s">
         <v>79</v>
@@ -3128,7 +3155,7 @@
       <c r="AG29" s="27"/>
     </row>
     <row r="30" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="12"/>
       <c r="C30" s="20" t="s">
         <v>77</v>
@@ -3171,7 +3198,7 @@
       <c r="AG30" s="27"/>
     </row>
     <row r="31" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="12"/>
       <c r="C31" s="19" t="s">
         <v>79</v>
@@ -3215,7 +3242,7 @@
     </row>
     <row r="32" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="17" t="s">
@@ -3264,7 +3291,7 @@
       <c r="AG33" s="27"/>
     </row>
     <row r="34" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="17" t="s">
         <v>96</v>
       </c>
@@ -3311,7 +3338,7 @@
       <c r="AG34" s="27"/>
     </row>
     <row r="35" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="17"/>
       <c r="C35" s="19" t="s">
         <v>79</v>
@@ -3354,7 +3381,7 @@
       <c r="AG35" s="27"/>
     </row>
     <row r="36" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="17"/>
       <c r="C36" s="19" t="s">
         <v>79</v>
@@ -3397,7 +3424,7 @@
       <c r="AG36" s="27"/>
     </row>
     <row r="37" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="17"/>
       <c r="C37" s="19" t="s">
         <v>79</v>
@@ -3440,7 +3467,7 @@
       <c r="AG37" s="27"/>
     </row>
     <row r="38" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="17"/>
       <c r="C38" s="19" t="s">
         <v>79</v>
@@ -3540,7 +3567,7 @@
       <c r="S40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T40" s="14" t="s">
+      <c r="T40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U40" s="14" t="s">
@@ -3639,7 +3666,7 @@
       <c r="S41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T41" s="14" t="s">
+      <c r="T41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U41" s="14" t="s">
@@ -3730,7 +3757,7 @@
       <c r="S42" s="26">
         <v>1</v>
       </c>
-      <c r="T42" s="14">
+      <c r="T42" s="26">
         <v>1</v>
       </c>
       <c r="U42" s="14">
@@ -3795,7 +3822,7 @@
       <c r="Q43" s="26"/>
       <c r="R43" s="26"/>
       <c r="S43" s="26"/>
-      <c r="T43" s="14"/>
+      <c r="T43" s="26"/>
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
       <c r="W43" s="14"/>
@@ -3836,7 +3863,7 @@
       <c r="Q44" s="26"/>
       <c r="R44" s="26"/>
       <c r="S44" s="26"/>
-      <c r="T44" s="14"/>
+      <c r="T44" s="26"/>
       <c r="U44" s="14"/>
       <c r="V44" s="14"/>
       <c r="W44" s="14"/>
@@ -3877,7 +3904,7 @@
       <c r="Q45" s="26"/>
       <c r="R45" s="26"/>
       <c r="S45" s="26"/>
-      <c r="T45" s="14"/>
+      <c r="T45" s="26"/>
       <c r="U45" s="14"/>
       <c r="V45" s="14"/>
       <c r="W45" s="14"/>
@@ -3893,7 +3920,7 @@
       <c r="AG45" s="14"/>
     </row>
     <row r="47" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -3944,7 +3971,7 @@
       <c r="AG47" s="27"/>
     </row>
     <row r="48" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="17" t="s">
         <v>96</v>
       </c>
@@ -3993,7 +4020,7 @@
       <c r="AG48" s="27"/>
     </row>
     <row r="49" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="17"/>
       <c r="C49" s="19" t="s">
         <v>79</v>
@@ -4040,7 +4067,7 @@
       <c r="AG49" s="27"/>
     </row>
     <row r="50" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="17"/>
       <c r="C50" s="19" t="s">
         <v>77</v>
@@ -4087,7 +4114,7 @@
       <c r="AG50" s="27"/>
     </row>
     <row r="51" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="17"/>
       <c r="C51" s="19" t="s">
         <v>79</v>
@@ -4134,7 +4161,7 @@
       <c r="AG51" s="27"/>
     </row>
     <row r="52" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="17"/>
       <c r="C52" s="19" t="s">
         <v>79</v>
@@ -4181,7 +4208,7 @@
       <c r="AG52" s="27"/>
     </row>
     <row r="53" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="17"/>
       <c r="C53" s="19" t="s">
         <v>77</v>
@@ -4228,7 +4255,7 @@
       <c r="AG53" s="27"/>
     </row>
     <row r="54" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
+      <c r="A54" s="35"/>
       <c r="B54" s="17"/>
       <c r="C54" s="19" t="s">
         <v>79</v>
@@ -4276,7 +4303,7 @@
     </row>
     <row r="55" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B56" s="17" t="s">
@@ -4335,7 +4362,7 @@
       <c r="AG56" s="27"/>
     </row>
     <row r="57" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="33"/>
+      <c r="A57" s="36"/>
       <c r="B57" s="17" t="s">
         <v>96</v>
       </c>
@@ -4392,7 +4419,7 @@
       <c r="AG57" s="27"/>
     </row>
     <row r="58" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="33"/>
+      <c r="A58" s="36"/>
       <c r="B58" s="17"/>
       <c r="C58" s="19" t="s">
         <v>79</v>
@@ -4437,7 +4464,7 @@
       <c r="AG58" s="27"/>
     </row>
     <row r="59" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="33"/>
+      <c r="A59" s="36"/>
       <c r="B59" s="17"/>
       <c r="C59" s="19" t="s">
         <v>79</v>
@@ -4484,7 +4511,7 @@
       <c r="AG59" s="27"/>
     </row>
     <row r="60" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="33"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="17"/>
       <c r="C60" s="19" t="s">
         <v>79</v>
@@ -4527,7 +4554,7 @@
       <c r="AG60" s="27"/>
     </row>
     <row r="61" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+      <c r="A61" s="36"/>
       <c r="B61" s="17"/>
       <c r="C61" s="19" t="s">
         <v>79</v>
@@ -4570,7 +4597,7 @@
       <c r="AG61" s="27"/>
     </row>
     <row r="62" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="17"/>
       <c r="C62" s="19" t="s">
         <v>79</v>
@@ -4613,7 +4640,7 @@
       <c r="AG62" s="27"/>
     </row>
     <row r="63" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="17"/>
       <c r="C63" s="19" t="s">
         <v>79</v>
@@ -4656,7 +4683,7 @@
       <c r="AG63" s="27"/>
     </row>
     <row r="64" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
+      <c r="A64" s="36"/>
       <c r="B64" s="17"/>
       <c r="C64" s="19" t="s">
         <v>79</v>
@@ -4699,7 +4726,7 @@
       <c r="AG64" s="27"/>
     </row>
     <row r="65" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
+      <c r="A65" s="36"/>
       <c r="B65" s="17"/>
       <c r="C65" s="19" t="s">
         <v>79</v>
@@ -4742,7 +4769,7 @@
       <c r="AG65" s="27"/>
     </row>
     <row r="66" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="17"/>
       <c r="C66" s="19" t="s">
         <v>79</v>
@@ -4787,7 +4814,7 @@
       <c r="AG66" s="27"/>
     </row>
     <row r="67" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="33"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="17"/>
       <c r="C67" s="19" t="s">
         <v>79</v>
@@ -4834,7 +4861,7 @@
       <c r="AG67" s="27"/>
     </row>
     <row r="68" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="33"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="17"/>
       <c r="C68" s="19" t="s">
         <v>79</v>
@@ -4881,7 +4908,7 @@
       <c r="AG68" s="27"/>
     </row>
     <row r="70" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B70" s="22"/>
@@ -4910,7 +4937,7 @@
       <c r="S70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T70" s="14" t="s">
+      <c r="T70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U70" s="14" t="s">
@@ -4954,7 +4981,7 @@
       </c>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A71" s="38"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="23"/>
       <c r="C71" s="21" t="s">
         <v>77</v>
@@ -4981,7 +5008,7 @@
       <c r="S71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="T71" s="14" t="s">
+      <c r="T71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="U71" s="14" t="s">
@@ -5025,7 +5052,7 @@
       </c>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A72" s="38"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="23"/>
       <c r="C72" s="21" t="s">
         <v>79</v>
@@ -5052,7 +5079,7 @@
       <c r="S72" s="26">
         <v>4</v>
       </c>
-      <c r="T72" s="14">
+      <c r="T72" s="26">
         <v>4</v>
       </c>
       <c r="U72" s="14">
@@ -5090,7 +5117,7 @@
       <c r="AG72" s="14"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A73" s="38"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="23"/>
       <c r="C73" s="21" t="s">
         <v>79</v>
@@ -5117,7 +5144,7 @@
       <c r="S73" s="26">
         <v>5</v>
       </c>
-      <c r="T73" s="14">
+      <c r="T73" s="26">
         <v>5</v>
       </c>
       <c r="U73" s="14">
@@ -5159,7 +5186,7 @@
       <c r="AG73" s="14"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A74" s="38"/>
+      <c r="A74" s="32"/>
       <c r="B74" s="23"/>
       <c r="C74" s="21" t="s">
         <v>79</v>
@@ -5184,7 +5211,7 @@
       <c r="Q74" s="27"/>
       <c r="R74" s="27"/>
       <c r="S74" s="26"/>
-      <c r="T74" s="14"/>
+      <c r="T74" s="26"/>
       <c r="U74" s="14"/>
       <c r="V74" s="14"/>
       <c r="W74" s="14"/>
@@ -5202,7 +5229,7 @@
       <c r="AG74" s="14"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A75" s="38"/>
+      <c r="A75" s="32"/>
       <c r="B75" s="23"/>
       <c r="C75" s="21" t="s">
         <v>79</v>
@@ -5227,7 +5254,7 @@
       <c r="Q75" s="27"/>
       <c r="R75" s="27"/>
       <c r="S75" s="26"/>
-      <c r="T75" s="14"/>
+      <c r="T75" s="26"/>
       <c r="U75" s="14"/>
       <c r="V75" s="14"/>
       <c r="W75" s="14"/>
@@ -5249,7 +5276,7 @@
       <c r="AG75" s="14"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A76" s="38"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="23"/>
       <c r="C76" s="21" t="s">
         <v>79</v>
@@ -5274,7 +5301,7 @@
       <c r="Q76" s="27"/>
       <c r="R76" s="27"/>
       <c r="S76" s="26"/>
-      <c r="T76" s="14"/>
+      <c r="T76" s="26"/>
       <c r="U76" s="14"/>
       <c r="V76" s="14"/>
       <c r="W76" s="14"/>
@@ -5294,7 +5321,7 @@
       <c r="AG76" s="14"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A77" s="38"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="23"/>
       <c r="C77" s="21" t="s">
         <v>79</v>
@@ -5319,7 +5346,7 @@
       <c r="Q77" s="27"/>
       <c r="R77" s="27"/>
       <c r="S77" s="26"/>
-      <c r="T77" s="14"/>
+      <c r="T77" s="26"/>
       <c r="U77" s="14"/>
       <c r="V77" s="14"/>
       <c r="W77" s="14"/>
@@ -5339,7 +5366,7 @@
       <c r="AG77" s="14"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A78" s="38"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="23"/>
       <c r="C78" s="21" t="s">
         <v>79</v>
@@ -5364,7 +5391,7 @@
       <c r="Q78" s="27"/>
       <c r="R78" s="27"/>
       <c r="S78" s="26"/>
-      <c r="T78" s="14"/>
+      <c r="T78" s="26"/>
       <c r="U78" s="14"/>
       <c r="V78" s="14"/>
       <c r="W78" s="14"/>
@@ -5382,7 +5409,7 @@
       <c r="AG78" s="14"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A79" s="38"/>
+      <c r="A79" s="32"/>
       <c r="B79" s="23"/>
       <c r="C79" s="21" t="s">
         <v>79</v>
@@ -5407,7 +5434,7 @@
       <c r="Q79" s="27"/>
       <c r="R79" s="27"/>
       <c r="S79" s="26"/>
-      <c r="T79" s="14"/>
+      <c r="T79" s="26"/>
       <c r="U79" s="14"/>
       <c r="V79" s="14"/>
       <c r="W79" s="14"/>
@@ -5425,7 +5452,7 @@
       <c r="AG79" s="14"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A80" s="38"/>
+      <c r="A80" s="32"/>
       <c r="B80" s="23"/>
       <c r="C80" s="21" t="s">
         <v>79</v>
@@ -5452,7 +5479,7 @@
       <c r="S80" s="26">
         <v>8</v>
       </c>
-      <c r="T80" s="14"/>
+      <c r="T80" s="26"/>
       <c r="U80" s="14"/>
       <c r="V80" s="14"/>
       <c r="W80" s="14"/>
@@ -5468,7 +5495,7 @@
       <c r="AG80" s="14"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A81" s="39"/>
+      <c r="A81" s="33"/>
       <c r="B81" s="24"/>
       <c r="C81" s="21" t="s">
         <v>79</v>
@@ -5495,7 +5522,7 @@
       <c r="S81" s="26">
         <v>9</v>
       </c>
-      <c r="T81" s="14"/>
+      <c r="T81" s="26"/>
       <c r="U81" s="14"/>
       <c r="V81" s="14"/>
       <c r="W81" s="14"/>
@@ -5747,10 +5774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6287,6 +6314,62 @@
       </c>
       <c r="D37" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C41" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some other technical production were added
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94153D06-343E-46D5-A477-5C37E2B1ED91}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C47F6D-D5DB-4EFE-AA66-729F7C9130B7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="233">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -660,6 +660,72 @@
   </si>
   <si>
     <t>Producción técnica - Productos tecnológicos - Base de datos de referencia para investigación</t>
+  </si>
+  <si>
+    <t>Producción técnica - Diseño Industrial</t>
+  </si>
+  <si>
+    <t>Diseño Industrial</t>
+  </si>
+  <si>
+    <t>Producción técnica - Esquema de circuito integrado</t>
+  </si>
+  <si>
+    <t>Esquema de circuito integrado</t>
+  </si>
+  <si>
+    <t>Producción técnica - Innovaciones generadas de producción empresarial - Empresarial</t>
+  </si>
+  <si>
+    <t>Producción técnica - Innovaciones generadas de producción empresarial - Organizacional</t>
+  </si>
+  <si>
+    <t>nnovaciones generadas de producción empresarial - Organizacional</t>
+  </si>
+  <si>
+    <t>Innovaciones generadas de producción empresarial - Empresarial</t>
+  </si>
+  <si>
+    <t>Variedad animal</t>
+  </si>
+  <si>
+    <t>Producción técnica - Variedad animal</t>
+  </si>
+  <si>
+    <t>Producción técnica - Innovación de proceso o procedimiento</t>
+  </si>
+  <si>
+    <t>Innovaciones</t>
+  </si>
+  <si>
+    <t>Innovación de proceso o procedimiento</t>
+  </si>
+  <si>
+    <t>Producción técnica - Cartas, mapas o similares - Aerofotograma</t>
+  </si>
+  <si>
+    <t>Producción técnica - Cartas, mapas o similares - Carta</t>
+  </si>
+  <si>
+    <t>Producción técnica - Cartas, mapas o similares - Fotograma</t>
+  </si>
+  <si>
+    <t>Producción técnica - Cartas, mapas o similares - Mapa</t>
+  </si>
+  <si>
+    <t>Producción técnica - Cartas, mapas o similares - Otra</t>
+  </si>
+  <si>
+    <t>Aerofotograma</t>
+  </si>
+  <si>
+    <t>Carta</t>
+  </si>
+  <si>
+    <t>Fotograma</t>
+  </si>
+  <si>
+    <t>Mapa</t>
   </si>
 </sst>
 </file>
@@ -1388,11 +1454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70E6F07-A587-464B-AE84-05F19DCFB741}">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="K40" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB15" sqref="AB15:AC16"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,22 +1672,22 @@
       <c r="T3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="14" t="s">
+      <c r="U3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA3" s="14" t="s">
@@ -1639,7 +1705,7 @@
       <c r="AE3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AF3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG3" s="14" t="s">
@@ -1703,22 +1769,22 @@
       <c r="T4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X4" s="14" t="s">
+      <c r="U4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y4" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA4" s="14" t="s">
@@ -1736,7 +1802,7 @@
       <c r="AE4" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF4" s="14" t="s">
+      <c r="AF4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG4" s="14" t="s">
@@ -1800,22 +1866,22 @@
       <c r="T5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" s="14" t="s">
+      <c r="U5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="14" t="s">
+      <c r="Z5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA5" s="14" t="s">
@@ -1833,7 +1899,7 @@
       <c r="AE5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF5" s="14" t="s">
+      <c r="AF5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG5" s="14" t="s">
@@ -1893,22 +1959,22 @@
       <c r="T6" s="26">
         <v>3</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="26">
         <v>3</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="26">
         <v>3</v>
       </c>
-      <c r="W6" s="14">
+      <c r="W6" s="26">
         <v>3</v>
       </c>
-      <c r="X6" s="14">
+      <c r="X6" s="26">
         <v>3</v>
       </c>
       <c r="Y6" s="14">
         <v>3</v>
       </c>
-      <c r="Z6" s="14">
+      <c r="Z6" s="26">
         <v>3</v>
       </c>
       <c r="AA6" s="14">
@@ -1926,7 +1992,7 @@
       <c r="AE6" s="14">
         <v>3</v>
       </c>
-      <c r="AF6" s="14">
+      <c r="AF6" s="26">
         <v>3</v>
       </c>
       <c r="AG6" s="14">
@@ -1964,18 +2030,18 @@
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
       <c r="T7" s="26"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
       <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
+      <c r="Z7" s="26"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
       <c r="AC7" s="14"/>
       <c r="AD7" s="14"/>
       <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
+      <c r="AF7" s="26"/>
       <c r="AG7" s="14"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
@@ -2007,18 +2073,18 @@
       <c r="R8" s="26"/>
       <c r="S8" s="26"/>
       <c r="T8" s="26"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
       <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
+      <c r="Z8" s="26"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
       <c r="AC8" s="14"/>
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
+      <c r="AF8" s="26"/>
       <c r="AG8" s="14"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
@@ -2052,18 +2118,18 @@
       <c r="R9" s="26"/>
       <c r="S9" s="26"/>
       <c r="T9" s="26"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
       <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
+      <c r="Z9" s="26"/>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
       <c r="AC9" s="14"/>
       <c r="AD9" s="14"/>
       <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
+      <c r="AF9" s="26"/>
       <c r="AG9" s="14"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
@@ -2115,22 +2181,22 @@
       <c r="T10" s="26">
         <v>6</v>
       </c>
-      <c r="U10" s="14">
+      <c r="U10" s="26">
         <v>6</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="26">
         <v>6</v>
       </c>
-      <c r="W10" s="14">
+      <c r="W10" s="26">
         <v>6</v>
       </c>
-      <c r="X10" s="14">
+      <c r="X10" s="26">
         <v>6</v>
       </c>
       <c r="Y10" s="14">
         <v>8</v>
       </c>
-      <c r="Z10" s="14">
+      <c r="Z10" s="26">
         <v>6</v>
       </c>
       <c r="AA10" s="14">
@@ -2146,7 +2212,7 @@
         <v>2</v>
       </c>
       <c r="AE10" s="14"/>
-      <c r="AF10" s="14">
+      <c r="AF10" s="26">
         <v>6</v>
       </c>
       <c r="AG10" s="14">
@@ -2202,22 +2268,22 @@
       <c r="T11" s="26">
         <v>7</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U11" s="26">
         <v>7</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="26">
         <v>7</v>
       </c>
-      <c r="W11" s="14">
+      <c r="W11" s="26">
         <v>7</v>
       </c>
-      <c r="X11" s="14">
+      <c r="X11" s="26">
         <v>7</v>
       </c>
       <c r="Y11" s="14">
         <v>9</v>
       </c>
-      <c r="Z11" s="14">
+      <c r="Z11" s="26">
         <v>7</v>
       </c>
       <c r="AA11" s="14">
@@ -2235,7 +2301,7 @@
       <c r="AE11" s="14">
         <v>5</v>
       </c>
-      <c r="AF11" s="14">
+      <c r="AF11" s="26">
         <v>7</v>
       </c>
       <c r="AG11" s="14">
@@ -2271,18 +2337,18 @@
       <c r="R12" s="26"/>
       <c r="S12" s="26"/>
       <c r="T12" s="26"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
       <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
+      <c r="Z12" s="26"/>
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
       <c r="AC12" s="14"/>
       <c r="AD12" s="14"/>
       <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
+      <c r="AF12" s="26"/>
       <c r="AG12" s="14"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -2328,22 +2394,22 @@
       <c r="T13" s="26">
         <v>8</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="26">
         <v>8</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="26">
         <v>8</v>
       </c>
-      <c r="W13" s="14">
+      <c r="W13" s="26">
         <v>8</v>
       </c>
-      <c r="X13" s="14">
+      <c r="X13" s="26">
         <v>8</v>
       </c>
       <c r="Y13" s="14">
         <v>10</v>
       </c>
-      <c r="Z13" s="14">
+      <c r="Z13" s="26">
         <v>8</v>
       </c>
       <c r="AA13" s="14">
@@ -2359,7 +2425,7 @@
       <c r="AE13" s="14">
         <v>6</v>
       </c>
-      <c r="AF13" s="14">
+      <c r="AF13" s="26">
         <v>8</v>
       </c>
       <c r="AG13" s="14"/>
@@ -2405,22 +2471,22 @@
       <c r="T14" s="26">
         <v>9</v>
       </c>
-      <c r="U14" s="14">
+      <c r="U14" s="26">
         <v>9</v>
       </c>
-      <c r="V14" s="14">
+      <c r="V14" s="26">
         <v>9</v>
       </c>
-      <c r="W14" s="14">
+      <c r="W14" s="26">
         <v>9</v>
       </c>
-      <c r="X14" s="14">
+      <c r="X14" s="26">
         <v>9</v>
       </c>
       <c r="Y14" s="14">
         <v>11</v>
       </c>
-      <c r="Z14" s="14">
+      <c r="Z14" s="26">
         <v>9</v>
       </c>
       <c r="AA14" s="14">
@@ -2436,7 +2502,7 @@
       <c r="AE14" s="14">
         <v>7</v>
       </c>
-      <c r="AF14" s="14">
+      <c r="AF14" s="26">
         <v>9</v>
       </c>
       <c r="AG14" s="14"/>
@@ -2478,22 +2544,22 @@
       <c r="T15" s="26">
         <v>10</v>
       </c>
-      <c r="U15" s="14">
+      <c r="U15" s="26">
         <v>10</v>
       </c>
-      <c r="V15" s="14">
+      <c r="V15" s="26">
         <v>10</v>
       </c>
-      <c r="W15" s="14">
+      <c r="W15" s="26">
         <v>10</v>
       </c>
-      <c r="X15" s="14">
+      <c r="X15" s="26">
         <v>10</v>
       </c>
       <c r="Y15" s="14">
         <v>12</v>
       </c>
-      <c r="Z15" s="14">
+      <c r="Z15" s="26">
         <v>10</v>
       </c>
       <c r="AA15" s="14">
@@ -2509,7 +2575,7 @@
       <c r="AE15" s="14">
         <v>8</v>
       </c>
-      <c r="AF15" s="14">
+      <c r="AF15" s="26">
         <v>10</v>
       </c>
       <c r="AG15" s="14"/>
@@ -2561,22 +2627,22 @@
       <c r="T16" s="26">
         <v>2</v>
       </c>
-      <c r="U16" s="14">
+      <c r="U16" s="26">
         <v>2</v>
       </c>
-      <c r="V16" s="14">
+      <c r="V16" s="26">
         <v>2</v>
       </c>
-      <c r="W16" s="14">
+      <c r="W16" s="26">
         <v>2</v>
       </c>
-      <c r="X16" s="14">
+      <c r="X16" s="26">
         <v>2</v>
       </c>
       <c r="Y16" s="14">
         <v>2</v>
       </c>
-      <c r="Z16" s="14">
+      <c r="Z16" s="26">
         <v>2</v>
       </c>
       <c r="AA16" s="14">
@@ -2592,7 +2658,7 @@
       <c r="AE16" s="14">
         <v>2</v>
       </c>
-      <c r="AF16" s="14">
+      <c r="AF16" s="26">
         <v>2</v>
       </c>
       <c r="AG16" s="14">
@@ -2628,18 +2694,18 @@
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
       <c r="T17" s="26"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="26"/>
       <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
+      <c r="Z17" s="26"/>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
       <c r="AC17" s="14"/>
       <c r="AD17" s="14"/>
       <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
+      <c r="AF17" s="26"/>
       <c r="AG17" s="14"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
@@ -2675,12 +2741,12 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
       <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
+      <c r="Z18" s="26"/>
       <c r="AA18" s="14"/>
       <c r="AB18" s="14">
         <v>8</v>
@@ -2690,7 +2756,7 @@
       </c>
       <c r="AD18" s="14"/>
       <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
+      <c r="AF18" s="26"/>
       <c r="AG18" s="14"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
@@ -2730,18 +2796,18 @@
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
       <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
+      <c r="Z19" s="26"/>
       <c r="AA19" s="14"/>
       <c r="AB19" s="14"/>
       <c r="AC19" s="14"/>
       <c r="AD19" s="14"/>
       <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
+      <c r="AF19" s="26"/>
       <c r="AG19" s="14"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
@@ -2779,12 +2845,12 @@
       </c>
       <c r="S20" s="26"/>
       <c r="T20" s="26"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
       <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
+      <c r="Z20" s="26"/>
       <c r="AA20" s="14">
         <v>9</v>
       </c>
@@ -2796,7 +2862,7 @@
       </c>
       <c r="AD20" s="14"/>
       <c r="AE20" s="14"/>
-      <c r="AF20" s="14"/>
+      <c r="AF20" s="26"/>
       <c r="AG20" s="14"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
@@ -2828,18 +2894,18 @@
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
       <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
+      <c r="Z21" s="26"/>
       <c r="AA21" s="14"/>
       <c r="AB21" s="14"/>
       <c r="AC21" s="14"/>
       <c r="AD21" s="14"/>
       <c r="AE21" s="14"/>
-      <c r="AF21" s="14"/>
+      <c r="AF21" s="26"/>
       <c r="AG21" s="14"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
@@ -2869,18 +2935,18 @@
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
       <c r="T22" s="26"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
       <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
+      <c r="Z22" s="26"/>
       <c r="AA22" s="14"/>
       <c r="AB22" s="14"/>
       <c r="AC22" s="14"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
-      <c r="AF22" s="14"/>
+      <c r="AF22" s="26"/>
       <c r="AG22" s="14">
         <v>6</v>
       </c>
@@ -2918,18 +2984,18 @@
       <c r="R23" s="26"/>
       <c r="S23" s="26"/>
       <c r="T23" s="26"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
       <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
+      <c r="Z23" s="26"/>
       <c r="AA23" s="14"/>
       <c r="AB23" s="14"/>
       <c r="AC23" s="14"/>
       <c r="AD23" s="14"/>
       <c r="AE23" s="14"/>
-      <c r="AF23" s="14"/>
+      <c r="AF23" s="26"/>
       <c r="AG23" s="14"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
@@ -2961,18 +3027,18 @@
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
       <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
+      <c r="Z24" s="26"/>
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
       <c r="AC24" s="14"/>
       <c r="AD24" s="14"/>
       <c r="AE24" s="14"/>
-      <c r="AF24" s="14"/>
+      <c r="AF24" s="26"/>
       <c r="AG24" s="14"/>
     </row>
     <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3570,22 +3636,22 @@
       <c r="T40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X40" s="14" t="s">
+      <c r="U40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y40" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z40" s="14" t="s">
+      <c r="Z40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA40" s="14" t="s">
@@ -3603,7 +3669,7 @@
       <c r="AE40" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF40" s="14" t="s">
+      <c r="AF40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG40" s="14" t="s">
@@ -3669,22 +3735,22 @@
       <c r="T41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X41" s="14" t="s">
+      <c r="U41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y41" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z41" s="14" t="s">
+      <c r="Z41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA41" s="14" t="s">
@@ -3702,7 +3768,7 @@
       <c r="AE41" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF41" s="14" t="s">
+      <c r="AF41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG41" s="14" t="s">
@@ -3760,22 +3826,22 @@
       <c r="T42" s="26">
         <v>1</v>
       </c>
-      <c r="U42" s="14">
+      <c r="U42" s="26">
         <v>1</v>
       </c>
-      <c r="V42" s="14">
+      <c r="V42" s="26">
         <v>1</v>
       </c>
-      <c r="W42" s="14">
+      <c r="W42" s="26">
         <v>1</v>
       </c>
-      <c r="X42" s="14">
+      <c r="X42" s="26">
         <v>1</v>
       </c>
       <c r="Y42" s="14">
         <v>1</v>
       </c>
-      <c r="Z42" s="14">
+      <c r="Z42" s="26">
         <v>1</v>
       </c>
       <c r="AA42" s="14">
@@ -3791,7 +3857,7 @@
       <c r="AE42" s="14">
         <v>1</v>
       </c>
-      <c r="AF42" s="14">
+      <c r="AF42" s="26">
         <v>1</v>
       </c>
       <c r="AG42" s="14"/>
@@ -3823,18 +3889,18 @@
       <c r="R43" s="26"/>
       <c r="S43" s="26"/>
       <c r="T43" s="26"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
       <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
+      <c r="Z43" s="26"/>
       <c r="AA43" s="14"/>
       <c r="AB43" s="14"/>
       <c r="AC43" s="14"/>
       <c r="AD43" s="14"/>
       <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
+      <c r="AF43" s="26"/>
       <c r="AG43" s="14"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
@@ -3864,18 +3930,18 @@
       <c r="R44" s="26"/>
       <c r="S44" s="26"/>
       <c r="T44" s="26"/>
-      <c r="U44" s="14"/>
-      <c r="V44" s="14"/>
-      <c r="W44" s="14"/>
-      <c r="X44" s="14"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
       <c r="Y44" s="14"/>
-      <c r="Z44" s="14"/>
+      <c r="Z44" s="26"/>
       <c r="AA44" s="14"/>
       <c r="AB44" s="14"/>
       <c r="AC44" s="14"/>
       <c r="AD44" s="14"/>
       <c r="AE44" s="14"/>
-      <c r="AF44" s="14"/>
+      <c r="AF44" s="26"/>
       <c r="AG44" s="14"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
@@ -3905,18 +3971,18 @@
       <c r="R45" s="26"/>
       <c r="S45" s="26"/>
       <c r="T45" s="26"/>
-      <c r="U45" s="14"/>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="14"/>
+      <c r="U45" s="26"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
       <c r="Y45" s="14"/>
-      <c r="Z45" s="14"/>
+      <c r="Z45" s="26"/>
       <c r="AA45" s="14"/>
       <c r="AB45" s="14"/>
       <c r="AC45" s="14"/>
       <c r="AD45" s="14"/>
       <c r="AE45" s="14"/>
-      <c r="AF45" s="14"/>
+      <c r="AF45" s="26"/>
       <c r="AG45" s="14"/>
     </row>
     <row r="47" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4940,22 +5006,22 @@
       <c r="T70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X70" s="14" t="s">
+      <c r="U70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y70" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z70" s="14" t="s">
+      <c r="Z70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA70" s="14" t="s">
@@ -4973,7 +5039,7 @@
       <c r="AE70" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF70" s="14" t="s">
+      <c r="AF70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG70" s="14" t="s">
@@ -5011,22 +5077,22 @@
       <c r="T71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="U71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="V71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="X71" s="14" t="s">
+      <c r="U71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="W71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="X71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Y71" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="Z71" s="14" t="s">
+      <c r="Z71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AA71" s="14" t="s">
@@ -5044,7 +5110,7 @@
       <c r="AE71" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AF71" s="14" t="s">
+      <c r="AF71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AG71" s="14" t="s">
@@ -5082,22 +5148,22 @@
       <c r="T72" s="26">
         <v>4</v>
       </c>
-      <c r="U72" s="14">
+      <c r="U72" s="26">
         <v>4</v>
       </c>
-      <c r="V72" s="14">
+      <c r="V72" s="26">
         <v>4</v>
       </c>
-      <c r="W72" s="14">
+      <c r="W72" s="26">
         <v>4</v>
       </c>
-      <c r="X72" s="14">
+      <c r="X72" s="26">
         <v>4</v>
       </c>
       <c r="Y72" s="14">
         <v>6</v>
       </c>
-      <c r="Z72" s="14">
+      <c r="Z72" s="26">
         <v>4</v>
       </c>
       <c r="AA72" s="14">
@@ -5111,7 +5177,7 @@
       </c>
       <c r="AD72" s="14"/>
       <c r="AE72" s="14"/>
-      <c r="AF72" s="14">
+      <c r="AF72" s="26">
         <v>4</v>
       </c>
       <c r="AG72" s="14"/>
@@ -5147,22 +5213,22 @@
       <c r="T73" s="26">
         <v>5</v>
       </c>
-      <c r="U73" s="14">
+      <c r="U73" s="26">
         <v>5</v>
       </c>
-      <c r="V73" s="14">
+      <c r="V73" s="26">
         <v>5</v>
       </c>
-      <c r="W73" s="14">
+      <c r="W73" s="26">
         <v>5</v>
       </c>
-      <c r="X73" s="14">
+      <c r="X73" s="26">
         <v>5</v>
       </c>
       <c r="Y73" s="14">
         <v>7</v>
       </c>
-      <c r="Z73" s="14">
+      <c r="Z73" s="26">
         <v>5</v>
       </c>
       <c r="AA73" s="14">
@@ -5180,7 +5246,7 @@
       <c r="AE73" s="14">
         <v>4</v>
       </c>
-      <c r="AF73" s="14">
+      <c r="AF73" s="26">
         <v>5</v>
       </c>
       <c r="AG73" s="14"/>
@@ -5212,12 +5278,12 @@
       <c r="R74" s="27"/>
       <c r="S74" s="26"/>
       <c r="T74" s="26"/>
-      <c r="U74" s="14"/>
-      <c r="V74" s="14"/>
-      <c r="W74" s="14"/>
-      <c r="X74" s="14"/>
+      <c r="U74" s="26"/>
+      <c r="V74" s="26"/>
+      <c r="W74" s="26"/>
+      <c r="X74" s="26"/>
       <c r="Y74" s="14"/>
-      <c r="Z74" s="14"/>
+      <c r="Z74" s="26"/>
       <c r="AA74" s="14"/>
       <c r="AB74" s="14"/>
       <c r="AC74" s="14"/>
@@ -5225,7 +5291,7 @@
         <v>5</v>
       </c>
       <c r="AE74" s="14"/>
-      <c r="AF74" s="14"/>
+      <c r="AF74" s="26"/>
       <c r="AG74" s="14"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.25">
@@ -5255,12 +5321,12 @@
       <c r="R75" s="27"/>
       <c r="S75" s="26"/>
       <c r="T75" s="26"/>
-      <c r="U75" s="14"/>
-      <c r="V75" s="14"/>
-      <c r="W75" s="14"/>
-      <c r="X75" s="14"/>
+      <c r="U75" s="26"/>
+      <c r="V75" s="26"/>
+      <c r="W75" s="26"/>
+      <c r="X75" s="26"/>
       <c r="Y75" s="14"/>
-      <c r="Z75" s="14"/>
+      <c r="Z75" s="26"/>
       <c r="AA75" s="14">
         <v>8</v>
       </c>
@@ -5272,7 +5338,7 @@
       </c>
       <c r="AD75" s="14"/>
       <c r="AE75" s="14"/>
-      <c r="AF75" s="14"/>
+      <c r="AF75" s="26"/>
       <c r="AG75" s="14"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.25">
@@ -5302,12 +5368,12 @@
       <c r="R76" s="27"/>
       <c r="S76" s="26"/>
       <c r="T76" s="26"/>
-      <c r="U76" s="14"/>
-      <c r="V76" s="14"/>
-      <c r="W76" s="14"/>
-      <c r="X76" s="14"/>
+      <c r="U76" s="26"/>
+      <c r="V76" s="26"/>
+      <c r="W76" s="26"/>
+      <c r="X76" s="26"/>
       <c r="Y76" s="14"/>
-      <c r="Z76" s="14"/>
+      <c r="Z76" s="26"/>
       <c r="AA76" s="14"/>
       <c r="AB76" s="14">
         <v>11</v>
@@ -5317,7 +5383,7 @@
       </c>
       <c r="AD76" s="14"/>
       <c r="AE76" s="14"/>
-      <c r="AF76" s="14"/>
+      <c r="AF76" s="26"/>
       <c r="AG76" s="14"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.25">
@@ -5347,12 +5413,12 @@
       <c r="R77" s="27"/>
       <c r="S77" s="26"/>
       <c r="T77" s="26"/>
-      <c r="U77" s="14"/>
-      <c r="V77" s="14"/>
-      <c r="W77" s="14"/>
-      <c r="X77" s="14"/>
+      <c r="U77" s="26"/>
+      <c r="V77" s="26"/>
+      <c r="W77" s="26"/>
+      <c r="X77" s="26"/>
       <c r="Y77" s="14"/>
-      <c r="Z77" s="14"/>
+      <c r="Z77" s="26"/>
       <c r="AA77" s="14"/>
       <c r="AB77" s="14">
         <v>12</v>
@@ -5362,7 +5428,7 @@
       </c>
       <c r="AD77" s="14"/>
       <c r="AE77" s="14"/>
-      <c r="AF77" s="14"/>
+      <c r="AF77" s="26"/>
       <c r="AG77" s="14"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
@@ -5392,20 +5458,20 @@
       <c r="R78" s="27"/>
       <c r="S78" s="26"/>
       <c r="T78" s="26"/>
-      <c r="U78" s="14"/>
-      <c r="V78" s="14"/>
-      <c r="W78" s="14"/>
-      <c r="X78" s="14"/>
+      <c r="U78" s="26"/>
+      <c r="V78" s="26"/>
+      <c r="W78" s="26"/>
+      <c r="X78" s="26"/>
       <c r="Y78" s="14">
         <v>4</v>
       </c>
-      <c r="Z78" s="14"/>
+      <c r="Z78" s="26"/>
       <c r="AA78" s="14"/>
       <c r="AB78" s="14"/>
       <c r="AC78" s="14"/>
       <c r="AD78" s="14"/>
       <c r="AE78" s="14"/>
-      <c r="AF78" s="14"/>
+      <c r="AF78" s="26"/>
       <c r="AG78" s="14"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.25">
@@ -5435,20 +5501,20 @@
       <c r="R79" s="27"/>
       <c r="S79" s="26"/>
       <c r="T79" s="26"/>
-      <c r="U79" s="14"/>
-      <c r="V79" s="14"/>
-      <c r="W79" s="14"/>
-      <c r="X79" s="14"/>
+      <c r="U79" s="26"/>
+      <c r="V79" s="26"/>
+      <c r="W79" s="26"/>
+      <c r="X79" s="26"/>
       <c r="Y79" s="14">
         <v>5</v>
       </c>
-      <c r="Z79" s="14"/>
+      <c r="Z79" s="26"/>
       <c r="AA79" s="14"/>
       <c r="AB79" s="14"/>
       <c r="AC79" s="14"/>
       <c r="AD79" s="14"/>
       <c r="AE79" s="14"/>
-      <c r="AF79" s="14"/>
+      <c r="AF79" s="26"/>
       <c r="AG79" s="14"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.25">
@@ -5480,18 +5546,18 @@
         <v>8</v>
       </c>
       <c r="T80" s="26"/>
-      <c r="U80" s="14"/>
-      <c r="V80" s="14"/>
-      <c r="W80" s="14"/>
-      <c r="X80" s="14"/>
+      <c r="U80" s="26"/>
+      <c r="V80" s="26"/>
+      <c r="W80" s="26"/>
+      <c r="X80" s="26"/>
       <c r="Y80" s="14"/>
-      <c r="Z80" s="14"/>
+      <c r="Z80" s="26"/>
       <c r="AA80" s="14"/>
       <c r="AB80" s="14"/>
       <c r="AC80" s="14"/>
       <c r="AD80" s="14"/>
       <c r="AE80" s="14"/>
-      <c r="AF80" s="14"/>
+      <c r="AF80" s="26"/>
       <c r="AG80" s="14"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.25">
@@ -5523,18 +5589,18 @@
         <v>9</v>
       </c>
       <c r="T81" s="26"/>
-      <c r="U81" s="14"/>
-      <c r="V81" s="14"/>
-      <c r="W81" s="14"/>
-      <c r="X81" s="14"/>
+      <c r="U81" s="26"/>
+      <c r="V81" s="26"/>
+      <c r="W81" s="26"/>
+      <c r="X81" s="26"/>
       <c r="Y81" s="14"/>
-      <c r="Z81" s="14"/>
+      <c r="Z81" s="26"/>
       <c r="AA81" s="14"/>
       <c r="AB81" s="14"/>
       <c r="AC81" s="14"/>
       <c r="AD81" s="14"/>
       <c r="AE81" s="14"/>
-      <c r="AF81" s="14"/>
+      <c r="AF81" s="26"/>
       <c r="AG81" s="14"/>
     </row>
     <row r="83" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5774,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6370,6 +6436,160 @@
       </c>
       <c r="D41" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" t="s">
+        <v>217</v>
+      </c>
+      <c r="D44" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C45" t="s">
+        <v>218</v>
+      </c>
+      <c r="D45" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" t="s">
+        <v>223</v>
+      </c>
+      <c r="D47" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" t="s">
+        <v>229</v>
+      </c>
+      <c r="D48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" t="s">
+        <v>230</v>
+      </c>
+      <c r="D49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="C50" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" t="s">
+        <v>232</v>
+      </c>
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C52" t="s">
+        <v>199</v>
+      </c>
+      <c r="D52" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reglamentations were added to technical production
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C47F6D-D5DB-4EFE-AA66-729F7C9130B7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0A8AB8-4781-4011-BBE5-6D1AD16ADC42}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="266">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -726,6 +726,105 @@
   </si>
   <si>
     <t>Mapa</t>
+  </si>
+  <si>
+    <t>Producción técnica - Variedad vegetal</t>
+  </si>
+  <si>
+    <t>Variedad vegetal</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Servicios de proyectos de IDI</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Comercialización de tecnología</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Análisis de competitividad</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Informe técnico</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Otro</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Acciones de transferencia tecnológica</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Desarrollo de productos</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Implementación de sistemas de análisis</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Consultoría en artes,arquitectura y diseño</t>
+  </si>
+  <si>
+    <t>Servicios de proyectos de IDI</t>
+  </si>
+  <si>
+    <t>Comercialización de tecnología</t>
+  </si>
+  <si>
+    <t>Análisis de competitividad</t>
+  </si>
+  <si>
+    <t>Informe técnico</t>
+  </si>
+  <si>
+    <t>Acciones de transferencia tecnológica</t>
+  </si>
+  <si>
+    <t>Desarrollo de productos</t>
+  </si>
+  <si>
+    <t>Implementación de sistemas de análisis</t>
+  </si>
+  <si>
+    <t>Consultoría en artes,arquitectura y diseño</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Ambiental o de Salud</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Educativa</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Social</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Técnica</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Guía de práctica clínica</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Proyecto de ley</t>
+  </si>
+  <si>
+    <t>Ambiental o de Salud</t>
+  </si>
+  <si>
+    <t>Educativa</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Técnica</t>
+  </si>
+  <si>
+    <t>Proyecto de ley</t>
+  </si>
+  <si>
+    <t>Guia de práctica Clínica</t>
+  </si>
+  <si>
+    <t>Reglamento Técnico</t>
+  </si>
+  <si>
+    <t>Producción técnica - Reglamento Técnico</t>
   </si>
 </sst>
 </file>
@@ -1454,11 +1553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70E6F07-A587-464B-AE84-05F19DCFB741}">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8:H21"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,19 +1783,19 @@
       <c r="X3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Y3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC3" s="14" t="s">
+      <c r="AA3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD3" s="14" t="s">
@@ -1781,19 +1880,19 @@
       <c r="X4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Y4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC4" s="14" t="s">
+      <c r="AA4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD4" s="14" t="s">
@@ -1878,19 +1977,19 @@
       <c r="X5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="14" t="s">
+      <c r="Y5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC5" s="14" t="s">
+      <c r="AA5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD5" s="14" t="s">
@@ -1971,19 +2070,19 @@
       <c r="X6" s="26">
         <v>3</v>
       </c>
-      <c r="Y6" s="14">
+      <c r="Y6" s="26">
         <v>3</v>
       </c>
       <c r="Z6" s="26">
         <v>3</v>
       </c>
-      <c r="AA6" s="14">
+      <c r="AA6" s="26">
         <v>3</v>
       </c>
-      <c r="AB6" s="14">
+      <c r="AB6" s="26">
         <v>3</v>
       </c>
-      <c r="AC6" s="14">
+      <c r="AC6" s="26">
         <v>3</v>
       </c>
       <c r="AD6" s="14">
@@ -2034,11 +2133,11 @@
       <c r="V7" s="26"/>
       <c r="W7" s="26"/>
       <c r="X7" s="26"/>
-      <c r="Y7" s="14"/>
+      <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
       <c r="AD7" s="14"/>
       <c r="AE7" s="14"/>
       <c r="AF7" s="26"/>
@@ -2077,11 +2176,11 @@
       <c r="V8" s="26"/>
       <c r="W8" s="26"/>
       <c r="X8" s="26"/>
-      <c r="Y8" s="14"/>
+      <c r="Y8" s="26"/>
       <c r="Z8" s="26"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
       <c r="AD8" s="14"/>
       <c r="AE8" s="14"/>
       <c r="AF8" s="26"/>
@@ -2122,11 +2221,11 @@
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
       <c r="X9" s="26"/>
-      <c r="Y9" s="14"/>
+      <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
       <c r="AD9" s="14"/>
       <c r="AE9" s="14"/>
       <c r="AF9" s="26"/>
@@ -2193,19 +2292,19 @@
       <c r="X10" s="26">
         <v>6</v>
       </c>
-      <c r="Y10" s="14">
+      <c r="Y10" s="26">
         <v>8</v>
       </c>
       <c r="Z10" s="26">
         <v>6</v>
       </c>
-      <c r="AA10" s="14">
+      <c r="AA10" s="26">
         <v>6</v>
       </c>
-      <c r="AB10" s="14">
+      <c r="AB10" s="26">
         <v>6</v>
       </c>
-      <c r="AC10" s="14">
+      <c r="AC10" s="26">
         <v>6</v>
       </c>
       <c r="AD10" s="14">
@@ -2280,19 +2379,19 @@
       <c r="X11" s="26">
         <v>7</v>
       </c>
-      <c r="Y11" s="14">
+      <c r="Y11" s="26">
         <v>9</v>
       </c>
       <c r="Z11" s="26">
         <v>7</v>
       </c>
-      <c r="AA11" s="14">
+      <c r="AA11" s="26">
         <v>7</v>
       </c>
-      <c r="AB11" s="14">
+      <c r="AB11" s="26">
         <v>7</v>
       </c>
-      <c r="AC11" s="14">
+      <c r="AC11" s="26">
         <v>7</v>
       </c>
       <c r="AD11" s="14">
@@ -2341,11 +2440,11 @@
       <c r="V12" s="26"/>
       <c r="W12" s="26"/>
       <c r="X12" s="26"/>
-      <c r="Y12" s="14"/>
+      <c r="Y12" s="26"/>
       <c r="Z12" s="26"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
       <c r="AD12" s="14"/>
       <c r="AE12" s="14"/>
       <c r="AF12" s="26"/>
@@ -2406,19 +2505,19 @@
       <c r="X13" s="26">
         <v>8</v>
       </c>
-      <c r="Y13" s="14">
+      <c r="Y13" s="26">
         <v>10</v>
       </c>
       <c r="Z13" s="26">
         <v>8</v>
       </c>
-      <c r="AA13" s="14">
+      <c r="AA13" s="26">
         <v>10</v>
       </c>
-      <c r="AB13" s="14">
+      <c r="AB13" s="26">
         <v>13</v>
       </c>
-      <c r="AC13" s="14">
+      <c r="AC13" s="26">
         <v>13</v>
       </c>
       <c r="AD13" s="14"/>
@@ -2483,19 +2582,19 @@
       <c r="X14" s="26">
         <v>9</v>
       </c>
-      <c r="Y14" s="14">
+      <c r="Y14" s="26">
         <v>11</v>
       </c>
       <c r="Z14" s="26">
         <v>9</v>
       </c>
-      <c r="AA14" s="14">
+      <c r="AA14" s="26">
         <v>11</v>
       </c>
-      <c r="AB14" s="14">
+      <c r="AB14" s="26">
         <v>14</v>
       </c>
-      <c r="AC14" s="14">
+      <c r="AC14" s="26">
         <v>14</v>
       </c>
       <c r="AD14" s="14"/>
@@ -2556,19 +2655,19 @@
       <c r="X15" s="26">
         <v>10</v>
       </c>
-      <c r="Y15" s="14">
+      <c r="Y15" s="26">
         <v>12</v>
       </c>
       <c r="Z15" s="26">
         <v>10</v>
       </c>
-      <c r="AA15" s="14">
+      <c r="AA15" s="26">
         <v>12</v>
       </c>
-      <c r="AB15" s="14">
+      <c r="AB15" s="26">
         <v>15</v>
       </c>
-      <c r="AC15" s="14">
+      <c r="AC15" s="26">
         <v>15</v>
       </c>
       <c r="AD15" s="14"/>
@@ -2639,19 +2738,19 @@
       <c r="X16" s="26">
         <v>2</v>
       </c>
-      <c r="Y16" s="14">
+      <c r="Y16" s="26">
         <v>2</v>
       </c>
       <c r="Z16" s="26">
         <v>2</v>
       </c>
-      <c r="AA16" s="14">
+      <c r="AA16" s="26">
         <v>2</v>
       </c>
-      <c r="AB16" s="14">
+      <c r="AB16" s="26">
         <v>2</v>
       </c>
-      <c r="AC16" s="14">
+      <c r="AC16" s="26">
         <v>2</v>
       </c>
       <c r="AD16" s="14"/>
@@ -2698,11 +2797,11 @@
       <c r="V17" s="26"/>
       <c r="W17" s="26"/>
       <c r="X17" s="26"/>
-      <c r="Y17" s="14"/>
+      <c r="Y17" s="26"/>
       <c r="Z17" s="26"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="26"/>
       <c r="AD17" s="14"/>
       <c r="AE17" s="14"/>
       <c r="AF17" s="26"/>
@@ -2745,13 +2844,13 @@
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
-      <c r="Y18" s="14"/>
+      <c r="Y18" s="26"/>
       <c r="Z18" s="26"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14">
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26">
         <v>8</v>
       </c>
-      <c r="AC18" s="14">
+      <c r="AC18" s="26">
         <v>8</v>
       </c>
       <c r="AD18" s="14"/>
@@ -2800,11 +2899,11 @@
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
-      <c r="Y19" s="14"/>
+      <c r="Y19" s="26"/>
       <c r="Z19" s="26"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
       <c r="AD19" s="14"/>
       <c r="AE19" s="14"/>
       <c r="AF19" s="26"/>
@@ -2849,15 +2948,15 @@
       <c r="V20" s="26"/>
       <c r="W20" s="26"/>
       <c r="X20" s="26"/>
-      <c r="Y20" s="14"/>
+      <c r="Y20" s="26"/>
       <c r="Z20" s="26"/>
-      <c r="AA20" s="14">
+      <c r="AA20" s="26">
         <v>9</v>
       </c>
-      <c r="AB20" s="14">
+      <c r="AB20" s="26">
         <v>10</v>
       </c>
-      <c r="AC20" s="14">
+      <c r="AC20" s="26">
         <v>10</v>
       </c>
       <c r="AD20" s="14"/>
@@ -2898,11 +2997,11 @@
       <c r="V21" s="26"/>
       <c r="W21" s="26"/>
       <c r="X21" s="26"/>
-      <c r="Y21" s="14"/>
+      <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
-      <c r="AC21" s="14"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
       <c r="AD21" s="14"/>
       <c r="AE21" s="14"/>
       <c r="AF21" s="26"/>
@@ -2939,11 +3038,11 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
-      <c r="Y22" s="14"/>
+      <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
-      <c r="AA22" s="14"/>
-      <c r="AB22" s="14"/>
-      <c r="AC22" s="14"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
       <c r="AD22" s="14"/>
       <c r="AE22" s="14"/>
       <c r="AF22" s="26"/>
@@ -2988,11 +3087,11 @@
       <c r="V23" s="26"/>
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
-      <c r="Y23" s="14"/>
+      <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="14"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
       <c r="AD23" s="14"/>
       <c r="AE23" s="14"/>
       <c r="AF23" s="26"/>
@@ -3031,11 +3130,11 @@
       <c r="V24" s="26"/>
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
-      <c r="Y24" s="14"/>
+      <c r="Y24" s="26"/>
       <c r="Z24" s="26"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="14"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
       <c r="AD24" s="14"/>
       <c r="AE24" s="14"/>
       <c r="AF24" s="26"/>
@@ -3648,19 +3747,19 @@
       <c r="X40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y40" s="14" t="s">
+      <c r="Y40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC40" s="14" t="s">
+      <c r="AA40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD40" s="14" t="s">
@@ -3747,19 +3846,19 @@
       <c r="X41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y41" s="14" t="s">
+      <c r="Y41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC41" s="14" t="s">
+      <c r="AA41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD41" s="14" t="s">
@@ -3838,19 +3937,19 @@
       <c r="X42" s="26">
         <v>1</v>
       </c>
-      <c r="Y42" s="14">
+      <c r="Y42" s="26">
         <v>1</v>
       </c>
       <c r="Z42" s="26">
         <v>1</v>
       </c>
-      <c r="AA42" s="14">
+      <c r="AA42" s="26">
         <v>1</v>
       </c>
-      <c r="AB42" s="14">
+      <c r="AB42" s="26">
         <v>1</v>
       </c>
-      <c r="AC42" s="14">
+      <c r="AC42" s="26">
         <v>1</v>
       </c>
       <c r="AD42" s="14"/>
@@ -3893,11 +3992,11 @@
       <c r="V43" s="26"/>
       <c r="W43" s="26"/>
       <c r="X43" s="26"/>
-      <c r="Y43" s="14"/>
+      <c r="Y43" s="26"/>
       <c r="Z43" s="26"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
+      <c r="AA43" s="26"/>
+      <c r="AB43" s="26"/>
+      <c r="AC43" s="26"/>
       <c r="AD43" s="14"/>
       <c r="AE43" s="14"/>
       <c r="AF43" s="26"/>
@@ -3934,11 +4033,11 @@
       <c r="V44" s="26"/>
       <c r="W44" s="26"/>
       <c r="X44" s="26"/>
-      <c r="Y44" s="14"/>
+      <c r="Y44" s="26"/>
       <c r="Z44" s="26"/>
-      <c r="AA44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AC44" s="14"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
       <c r="AD44" s="14"/>
       <c r="AE44" s="14"/>
       <c r="AF44" s="26"/>
@@ -3975,11 +4074,11 @@
       <c r="V45" s="26"/>
       <c r="W45" s="26"/>
       <c r="X45" s="26"/>
-      <c r="Y45" s="14"/>
+      <c r="Y45" s="26"/>
       <c r="Z45" s="26"/>
-      <c r="AA45" s="14"/>
-      <c r="AB45" s="14"/>
-      <c r="AC45" s="14"/>
+      <c r="AA45" s="26"/>
+      <c r="AB45" s="26"/>
+      <c r="AC45" s="26"/>
       <c r="AD45" s="14"/>
       <c r="AE45" s="14"/>
       <c r="AF45" s="26"/>
@@ -5018,19 +5117,19 @@
       <c r="X70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y70" s="14" t="s">
+      <c r="Y70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC70" s="14" t="s">
+      <c r="AA70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD70" s="14" t="s">
@@ -5089,19 +5188,19 @@
       <c r="X71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="Y71" s="14" t="s">
+      <c r="Y71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="Z71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AA71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC71" s="14" t="s">
+      <c r="AA71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AD71" s="14" t="s">
@@ -5160,19 +5259,19 @@
       <c r="X72" s="26">
         <v>4</v>
       </c>
-      <c r="Y72" s="14">
+      <c r="Y72" s="26">
         <v>6</v>
       </c>
       <c r="Z72" s="26">
         <v>4</v>
       </c>
-      <c r="AA72" s="14">
+      <c r="AA72" s="26">
         <v>4</v>
       </c>
-      <c r="AB72" s="14">
+      <c r="AB72" s="26">
         <v>4</v>
       </c>
-      <c r="AC72" s="14">
+      <c r="AC72" s="26">
         <v>4</v>
       </c>
       <c r="AD72" s="14"/>
@@ -5225,19 +5324,19 @@
       <c r="X73" s="26">
         <v>5</v>
       </c>
-      <c r="Y73" s="14">
+      <c r="Y73" s="26">
         <v>7</v>
       </c>
       <c r="Z73" s="26">
         <v>5</v>
       </c>
-      <c r="AA73" s="14">
+      <c r="AA73" s="26">
         <v>5</v>
       </c>
-      <c r="AB73" s="14">
+      <c r="AB73" s="26">
         <v>5</v>
       </c>
-      <c r="AC73" s="14">
+      <c r="AC73" s="26">
         <v>5</v>
       </c>
       <c r="AD73" s="14">
@@ -5282,11 +5381,11 @@
       <c r="V74" s="26"/>
       <c r="W74" s="26"/>
       <c r="X74" s="26"/>
-      <c r="Y74" s="14"/>
+      <c r="Y74" s="26"/>
       <c r="Z74" s="26"/>
-      <c r="AA74" s="14"/>
-      <c r="AB74" s="14"/>
-      <c r="AC74" s="14"/>
+      <c r="AA74" s="26"/>
+      <c r="AB74" s="26"/>
+      <c r="AC74" s="26"/>
       <c r="AD74" s="14">
         <v>5</v>
       </c>
@@ -5325,15 +5424,15 @@
       <c r="V75" s="26"/>
       <c r="W75" s="26"/>
       <c r="X75" s="26"/>
-      <c r="Y75" s="14"/>
+      <c r="Y75" s="26"/>
       <c r="Z75" s="26"/>
-      <c r="AA75" s="14">
+      <c r="AA75" s="26">
         <v>8</v>
       </c>
-      <c r="AB75" s="14">
+      <c r="AB75" s="26">
         <v>9</v>
       </c>
-      <c r="AC75" s="14">
+      <c r="AC75" s="26">
         <v>9</v>
       </c>
       <c r="AD75" s="14"/>
@@ -5372,13 +5471,13 @@
       <c r="V76" s="26"/>
       <c r="W76" s="26"/>
       <c r="X76" s="26"/>
-      <c r="Y76" s="14"/>
+      <c r="Y76" s="26"/>
       <c r="Z76" s="26"/>
-      <c r="AA76" s="14"/>
-      <c r="AB76" s="14">
+      <c r="AA76" s="26"/>
+      <c r="AB76" s="26">
         <v>11</v>
       </c>
-      <c r="AC76" s="14">
+      <c r="AC76" s="26">
         <v>11</v>
       </c>
       <c r="AD76" s="14"/>
@@ -5417,13 +5516,13 @@
       <c r="V77" s="26"/>
       <c r="W77" s="26"/>
       <c r="X77" s="26"/>
-      <c r="Y77" s="14"/>
+      <c r="Y77" s="26"/>
       <c r="Z77" s="26"/>
-      <c r="AA77" s="14"/>
-      <c r="AB77" s="14">
+      <c r="AA77" s="26"/>
+      <c r="AB77" s="26">
         <v>12</v>
       </c>
-      <c r="AC77" s="14">
+      <c r="AC77" s="26">
         <v>12</v>
       </c>
       <c r="AD77" s="14"/>
@@ -5462,13 +5561,13 @@
       <c r="V78" s="26"/>
       <c r="W78" s="26"/>
       <c r="X78" s="26"/>
-      <c r="Y78" s="14">
+      <c r="Y78" s="26">
         <v>4</v>
       </c>
       <c r="Z78" s="26"/>
-      <c r="AA78" s="14"/>
-      <c r="AB78" s="14"/>
-      <c r="AC78" s="14"/>
+      <c r="AA78" s="26"/>
+      <c r="AB78" s="26"/>
+      <c r="AC78" s="26"/>
       <c r="AD78" s="14"/>
       <c r="AE78" s="14"/>
       <c r="AF78" s="26"/>
@@ -5505,13 +5604,13 @@
       <c r="V79" s="26"/>
       <c r="W79" s="26"/>
       <c r="X79" s="26"/>
-      <c r="Y79" s="14">
+      <c r="Y79" s="26">
         <v>5</v>
       </c>
       <c r="Z79" s="26"/>
-      <c r="AA79" s="14"/>
-      <c r="AB79" s="14"/>
-      <c r="AC79" s="14"/>
+      <c r="AA79" s="26"/>
+      <c r="AB79" s="26"/>
+      <c r="AC79" s="26"/>
       <c r="AD79" s="14"/>
       <c r="AE79" s="14"/>
       <c r="AF79" s="26"/>
@@ -5550,11 +5649,11 @@
       <c r="V80" s="26"/>
       <c r="W80" s="26"/>
       <c r="X80" s="26"/>
-      <c r="Y80" s="14"/>
+      <c r="Y80" s="26"/>
       <c r="Z80" s="26"/>
-      <c r="AA80" s="14"/>
-      <c r="AB80" s="14"/>
-      <c r="AC80" s="14"/>
+      <c r="AA80" s="26"/>
+      <c r="AB80" s="26"/>
+      <c r="AC80" s="26"/>
       <c r="AD80" s="14"/>
       <c r="AE80" s="14"/>
       <c r="AF80" s="26"/>
@@ -5593,11 +5692,11 @@
       <c r="V81" s="26"/>
       <c r="W81" s="26"/>
       <c r="X81" s="26"/>
-      <c r="Y81" s="14"/>
+      <c r="Y81" s="26"/>
       <c r="Z81" s="26"/>
-      <c r="AA81" s="14"/>
-      <c r="AB81" s="14"/>
-      <c r="AC81" s="14"/>
+      <c r="AA81" s="26"/>
+      <c r="AB81" s="26"/>
+      <c r="AC81" s="26"/>
       <c r="AD81" s="14"/>
       <c r="AE81" s="14"/>
       <c r="AF81" s="26"/>
@@ -5840,10 +5939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,6 +6688,244 @@
         <v>199</v>
       </c>
       <c r="D52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" t="s">
+        <v>234</v>
+      </c>
+      <c r="D53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" t="s">
+        <v>244</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" t="s">
+        <v>245</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" t="s">
+        <v>246</v>
+      </c>
+      <c r="D56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" t="s">
+        <v>247</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" t="s">
+        <v>248</v>
+      </c>
+      <c r="D59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" t="s">
+        <v>249</v>
+      </c>
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" t="s">
+        <v>250</v>
+      </c>
+      <c r="D61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" t="s">
+        <v>251</v>
+      </c>
+      <c r="D62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="C63" t="s">
+        <v>258</v>
+      </c>
+      <c r="D63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="C64" t="s">
+        <v>259</v>
+      </c>
+      <c r="D64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>254</v>
+      </c>
+      <c r="C65" t="s">
+        <v>260</v>
+      </c>
+      <c r="D65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C66" t="s">
+        <v>261</v>
+      </c>
+      <c r="D66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C67" t="s">
+        <v>263</v>
+      </c>
+      <c r="D67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="C68" t="s">
+        <v>262</v>
+      </c>
+      <c r="D68" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C69" t="s">
+        <v>264</v>
+      </c>
+      <c r="D69" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final version for Technical Production
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0A8AB8-4781-4011-BBE5-6D1AD16ADC42}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1483552-A794-43DF-A8EA-DF73DAC71AA7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="286">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -659,9 +659,6 @@
     <t>Productos Tecnológicos</t>
   </si>
   <si>
-    <t>Producción técnica - Productos tecnológicos - Base de datos de referencia para investigación</t>
-  </si>
-  <si>
     <t>Producción técnica - Diseño Industrial</t>
   </si>
   <si>
@@ -825,6 +822,69 @@
   </si>
   <si>
     <t>Producción técnica - Reglamento Técnico</t>
+  </si>
+  <si>
+    <t>Producción técnica - Empresa de base tecnológica - Spin-off</t>
+  </si>
+  <si>
+    <t>Producción técnica - Empresa de base tecnológica - Start-up</t>
+  </si>
+  <si>
+    <t>Empresa de base tecnológica - Spin-off</t>
+  </si>
+  <si>
+    <t>Empresa de base tecnológica - Start-up</t>
+  </si>
+  <si>
+    <t>Demás trabajos - Demás trabajos</t>
+  </si>
+  <si>
+    <t>Demás trabajos</t>
+  </si>
+  <si>
+    <t>Producción técnica - Signos</t>
+  </si>
+  <si>
+    <t>Signos</t>
+  </si>
+  <si>
+    <t>Producción técnica - Softwares - Multimedia</t>
+  </si>
+  <si>
+    <t>Multimedia</t>
+  </si>
+  <si>
+    <t>Producción técnica - Softwares - Otra</t>
+  </si>
+  <si>
+    <t>Softwares - Otra</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Técnica - Básica</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Técnica - Ensayo</t>
+  </si>
+  <si>
+    <t>Técnica - Ensayo</t>
+  </si>
+  <si>
+    <t>Técnica - Básica</t>
+  </si>
+  <si>
+    <t>Producción técnica - Consultoría Científico Tecnológica e Informe Técnico - Servicios de Proyectos de I+D+I</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Servicios de Proyectos de I+D+I</t>
+  </si>
+  <si>
+    <t>Producción técnica - Regulación, norma, reglamento o legislación - Técnica - Proceso</t>
+  </si>
+  <si>
+    <t>Producción técnica - Productos tecnológicos - Base de datos de referencia para investigacion</t>
+  </si>
+  <si>
+    <t>Técnica - Proceso</t>
   </si>
 </sst>
 </file>
@@ -1553,19 +1613,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70E6F07-A587-464B-AE84-05F19DCFB741}">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="18" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="18" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="33" width="4.42578125" style="15" customWidth="1"/>
   </cols>
@@ -1726,9 +1786,7 @@
       <c r="E3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="F3" s="14"/>
       <c r="G3" s="14" t="s">
         <v>55</v>
       </c>
@@ -1798,16 +1856,16 @@
       <c r="AC3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AD3" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG3" s="14" t="s">
+      <c r="AG3" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1895,16 +1953,16 @@
       <c r="AC4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE4" s="14" t="s">
+      <c r="AD4" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG4" s="14" t="s">
+      <c r="AG4" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1992,16 +2050,16 @@
       <c r="AC5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD5" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE5" s="14" t="s">
+      <c r="AD5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE5" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="14" t="s">
+      <c r="AG5" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2085,16 +2143,16 @@
       <c r="AC6" s="26">
         <v>3</v>
       </c>
-      <c r="AD6" s="14">
+      <c r="AD6" s="26">
         <v>1</v>
       </c>
-      <c r="AE6" s="14">
+      <c r="AE6" s="26">
         <v>3</v>
       </c>
       <c r="AF6" s="26">
         <v>3</v>
       </c>
-      <c r="AG6" s="14">
+      <c r="AG6" s="26">
         <v>3</v>
       </c>
     </row>
@@ -2138,10 +2196,10 @@
       <c r="AA7" s="26"/>
       <c r="AB7" s="26"/>
       <c r="AC7" s="26"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
       <c r="AF7" s="26"/>
-      <c r="AG7" s="14"/>
+      <c r="AG7" s="26"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
@@ -2181,10 +2239,10 @@
       <c r="AA8" s="26"/>
       <c r="AB8" s="26"/>
       <c r="AC8" s="26"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
       <c r="AF8" s="26"/>
-      <c r="AG8" s="14"/>
+      <c r="AG8" s="26"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
@@ -2226,10 +2284,10 @@
       <c r="AA9" s="26"/>
       <c r="AB9" s="26"/>
       <c r="AC9" s="26"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
       <c r="AF9" s="26"/>
-      <c r="AG9" s="14"/>
+      <c r="AG9" s="26"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
@@ -2307,14 +2365,14 @@
       <c r="AC10" s="26">
         <v>6</v>
       </c>
-      <c r="AD10" s="14">
+      <c r="AD10" s="26">
         <v>2</v>
       </c>
-      <c r="AE10" s="14"/>
+      <c r="AE10" s="26"/>
       <c r="AF10" s="26">
         <v>6</v>
       </c>
-      <c r="AG10" s="14">
+      <c r="AG10" s="26">
         <v>4</v>
       </c>
     </row>
@@ -2394,16 +2452,16 @@
       <c r="AC11" s="26">
         <v>7</v>
       </c>
-      <c r="AD11" s="14">
+      <c r="AD11" s="26">
         <v>3</v>
       </c>
-      <c r="AE11" s="14">
+      <c r="AE11" s="26">
         <v>5</v>
       </c>
       <c r="AF11" s="26">
         <v>7</v>
       </c>
-      <c r="AG11" s="14">
+      <c r="AG11" s="26">
         <v>5</v>
       </c>
     </row>
@@ -2445,10 +2503,10 @@
       <c r="AA12" s="26"/>
       <c r="AB12" s="26"/>
       <c r="AC12" s="26"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
       <c r="AF12" s="26"/>
-      <c r="AG12" s="14"/>
+      <c r="AG12" s="26"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
@@ -2520,14 +2578,14 @@
       <c r="AC13" s="26">
         <v>13</v>
       </c>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14">
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26">
         <v>6</v>
       </c>
       <c r="AF13" s="26">
         <v>8</v>
       </c>
-      <c r="AG13" s="14"/>
+      <c r="AG13" s="26"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
@@ -2597,14 +2655,14 @@
       <c r="AC14" s="26">
         <v>14</v>
       </c>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14">
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26">
         <v>7</v>
       </c>
       <c r="AF14" s="26">
         <v>9</v>
       </c>
-      <c r="AG14" s="14"/>
+      <c r="AG14" s="26"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
@@ -2670,14 +2728,14 @@
       <c r="AC15" s="26">
         <v>15</v>
       </c>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14">
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26">
         <v>8</v>
       </c>
       <c r="AF15" s="26">
         <v>10</v>
       </c>
-      <c r="AG15" s="14"/>
+      <c r="AG15" s="26"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
@@ -2753,14 +2811,14 @@
       <c r="AC16" s="26">
         <v>2</v>
       </c>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14">
+      <c r="AD16" s="26"/>
+      <c r="AE16" s="26">
         <v>2</v>
       </c>
       <c r="AF16" s="26">
         <v>2</v>
       </c>
-      <c r="AG16" s="14">
+      <c r="AG16" s="26">
         <v>2</v>
       </c>
     </row>
@@ -2802,10 +2860,10 @@
       <c r="AA17" s="26"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
+      <c r="AD17" s="26"/>
+      <c r="AE17" s="26"/>
       <c r="AF17" s="26"/>
-      <c r="AG17" s="14"/>
+      <c r="AG17" s="26"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
@@ -2853,10 +2911,10 @@
       <c r="AC18" s="26">
         <v>8</v>
       </c>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
+      <c r="AD18" s="26"/>
+      <c r="AE18" s="26"/>
       <c r="AF18" s="26"/>
-      <c r="AG18" s="14"/>
+      <c r="AG18" s="26"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
@@ -2904,10 +2962,10 @@
       <c r="AA19" s="26"/>
       <c r="AB19" s="26"/>
       <c r="AC19" s="26"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
+      <c r="AD19" s="26"/>
+      <c r="AE19" s="26"/>
       <c r="AF19" s="26"/>
-      <c r="AG19" s="14"/>
+      <c r="AG19" s="26"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
@@ -2959,10 +3017,10 @@
       <c r="AC20" s="26">
         <v>10</v>
       </c>
-      <c r="AD20" s="14"/>
-      <c r="AE20" s="14"/>
+      <c r="AD20" s="26"/>
+      <c r="AE20" s="26"/>
       <c r="AF20" s="26"/>
-      <c r="AG20" s="14"/>
+      <c r="AG20" s="26"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
@@ -3002,10 +3060,10 @@
       <c r="AA21" s="26"/>
       <c r="AB21" s="26"/>
       <c r="AC21" s="26"/>
-      <c r="AD21" s="14"/>
-      <c r="AE21" s="14"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="26"/>
       <c r="AF21" s="26"/>
-      <c r="AG21" s="14"/>
+      <c r="AG21" s="26"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
@@ -3043,10 +3101,10 @@
       <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
       <c r="AC22" s="26"/>
-      <c r="AD22" s="14"/>
-      <c r="AE22" s="14"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
       <c r="AF22" s="26"/>
-      <c r="AG22" s="14">
+      <c r="AG22" s="26">
         <v>6</v>
       </c>
     </row>
@@ -3092,10 +3150,10 @@
       <c r="AA23" s="26"/>
       <c r="AB23" s="26"/>
       <c r="AC23" s="26"/>
-      <c r="AD23" s="14"/>
-      <c r="AE23" s="14"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="26"/>
       <c r="AF23" s="26"/>
-      <c r="AG23" s="14"/>
+      <c r="AG23" s="26"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
@@ -3135,13 +3193,13 @@
       <c r="AA24" s="26"/>
       <c r="AB24" s="26"/>
       <c r="AC24" s="26"/>
-      <c r="AD24" s="14"/>
-      <c r="AE24" s="14"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
       <c r="AF24" s="26"/>
-      <c r="AG24" s="14"/>
+      <c r="AG24" s="26"/>
     </row>
     <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:33" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>53</v>
       </c>
@@ -3188,7 +3246,7 @@
       <c r="AF26" s="27"/>
       <c r="AG26" s="27"/>
     </row>
-    <row r="27" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="17" t="s">
         <v>96</v>
@@ -3233,7 +3291,7 @@
       <c r="AF27" s="27"/>
       <c r="AG27" s="27"/>
     </row>
-    <row r="28" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" s="12"/>
       <c r="C28" s="19" t="s">
@@ -3276,7 +3334,7 @@
       <c r="AF28" s="27"/>
       <c r="AG28" s="27"/>
     </row>
-    <row r="29" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="12"/>
       <c r="C29" s="19" t="s">
@@ -3319,7 +3377,7 @@
       <c r="AF29" s="27"/>
       <c r="AG29" s="27"/>
     </row>
-    <row r="30" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" s="12"/>
       <c r="C30" s="20" t="s">
@@ -3362,7 +3420,7 @@
       <c r="AF30" s="27"/>
       <c r="AG30" s="27"/>
     </row>
-    <row r="31" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" s="12"/>
       <c r="C31" s="19" t="s">
@@ -3405,8 +3463,7 @@
       <c r="AF31" s="27"/>
       <c r="AG31" s="27"/>
     </row>
-    <row r="32" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="38" t="s">
         <v>1</v>
       </c>
@@ -3455,7 +3512,7 @@
       <c r="AF33" s="27"/>
       <c r="AG33" s="27"/>
     </row>
-    <row r="34" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="38"/>
       <c r="B34" s="17" t="s">
         <v>96</v>
@@ -3502,7 +3559,7 @@
       <c r="AF34" s="27"/>
       <c r="AG34" s="27"/>
     </row>
-    <row r="35" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="38"/>
       <c r="B35" s="17"/>
       <c r="C35" s="19" t="s">
@@ -3545,7 +3602,7 @@
       <c r="AF35" s="27"/>
       <c r="AG35" s="27"/>
     </row>
-    <row r="36" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="38"/>
       <c r="B36" s="17"/>
       <c r="C36" s="19" t="s">
@@ -3588,7 +3645,7 @@
       <c r="AF36" s="27"/>
       <c r="AG36" s="27"/>
     </row>
-    <row r="37" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="38"/>
       <c r="B37" s="17"/>
       <c r="C37" s="19" t="s">
@@ -3631,7 +3688,7 @@
       <c r="AF37" s="27"/>
       <c r="AG37" s="27"/>
     </row>
-    <row r="38" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="38"/>
       <c r="B38" s="17"/>
       <c r="C38" s="19" t="s">
@@ -3690,9 +3747,7 @@
       <c r="E40" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="F40" s="14"/>
       <c r="G40" s="14" t="s">
         <v>55</v>
       </c>
@@ -3762,16 +3817,16 @@
       <c r="AC40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD40" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE40" s="14" t="s">
+      <c r="AD40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE40" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF40" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG40" s="14" t="s">
+      <c r="AG40" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3789,9 +3844,7 @@
       <c r="E41" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="F41" s="14"/>
       <c r="G41" s="14" t="s">
         <v>55</v>
       </c>
@@ -3861,16 +3914,16 @@
       <c r="AC41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD41" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE41" s="14" t="s">
+      <c r="AD41" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE41" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF41" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG41" s="14" t="s">
+      <c r="AG41" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3952,14 +4005,14 @@
       <c r="AC42" s="26">
         <v>1</v>
       </c>
-      <c r="AD42" s="14"/>
-      <c r="AE42" s="14">
+      <c r="AD42" s="26"/>
+      <c r="AE42" s="26">
         <v>1</v>
       </c>
       <c r="AF42" s="26">
         <v>1</v>
       </c>
-      <c r="AG42" s="14"/>
+      <c r="AG42" s="26"/>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
@@ -3997,10 +4050,10 @@
       <c r="AA43" s="26"/>
       <c r="AB43" s="26"/>
       <c r="AC43" s="26"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="14"/>
+      <c r="AD43" s="26"/>
+      <c r="AE43" s="26"/>
       <c r="AF43" s="26"/>
-      <c r="AG43" s="14"/>
+      <c r="AG43" s="26"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
@@ -4038,10 +4091,10 @@
       <c r="AA44" s="26"/>
       <c r="AB44" s="26"/>
       <c r="AC44" s="26"/>
-      <c r="AD44" s="14"/>
-      <c r="AE44" s="14"/>
+      <c r="AD44" s="26"/>
+      <c r="AE44" s="26"/>
       <c r="AF44" s="26"/>
-      <c r="AG44" s="14"/>
+      <c r="AG44" s="26"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
@@ -4079,12 +4132,12 @@
       <c r="AA45" s="26"/>
       <c r="AB45" s="26"/>
       <c r="AC45" s="26"/>
-      <c r="AD45" s="14"/>
-      <c r="AE45" s="14"/>
+      <c r="AD45" s="26"/>
+      <c r="AE45" s="26"/>
       <c r="AF45" s="26"/>
-      <c r="AG45" s="14"/>
-    </row>
-    <row r="47" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG45" s="26"/>
+    </row>
+    <row r="47" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>3</v>
       </c>
@@ -4135,7 +4188,7 @@
       <c r="AF47" s="27"/>
       <c r="AG47" s="27"/>
     </row>
-    <row r="48" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="35"/>
       <c r="B48" s="17" t="s">
         <v>96</v>
@@ -4184,7 +4237,7 @@
       <c r="AF48" s="27"/>
       <c r="AG48" s="27"/>
     </row>
-    <row r="49" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="35"/>
       <c r="B49" s="17"/>
       <c r="C49" s="19" t="s">
@@ -4231,7 +4284,7 @@
       <c r="AF49" s="27"/>
       <c r="AG49" s="27"/>
     </row>
-    <row r="50" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="17"/>
       <c r="C50" s="19" t="s">
@@ -4278,7 +4331,7 @@
       <c r="AF50" s="27"/>
       <c r="AG50" s="27"/>
     </row>
-    <row r="51" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="17"/>
       <c r="C51" s="19" t="s">
@@ -4325,7 +4378,7 @@
       <c r="AF51" s="27"/>
       <c r="AG51" s="27"/>
     </row>
-    <row r="52" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="35"/>
       <c r="B52" s="17"/>
       <c r="C52" s="19" t="s">
@@ -4372,7 +4425,7 @@
       <c r="AF52" s="27"/>
       <c r="AG52" s="27"/>
     </row>
-    <row r="53" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
       <c r="B53" s="17"/>
       <c r="C53" s="19" t="s">
@@ -4419,7 +4472,7 @@
       <c r="AF53" s="27"/>
       <c r="AG53" s="27"/>
     </row>
-    <row r="54" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
       <c r="B54" s="17"/>
       <c r="C54" s="19" t="s">
@@ -4466,8 +4519,7 @@
       <c r="AF54" s="27"/>
       <c r="AG54" s="27"/>
     </row>
-    <row r="55" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
         <v>86</v>
       </c>
@@ -4526,7 +4578,7 @@
       <c r="AF56" s="27"/>
       <c r="AG56" s="27"/>
     </row>
-    <row r="57" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="36"/>
       <c r="B57" s="17" t="s">
         <v>96</v>
@@ -4583,7 +4635,7 @@
       <c r="AF57" s="27"/>
       <c r="AG57" s="27"/>
     </row>
-    <row r="58" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" s="36"/>
       <c r="B58" s="17"/>
       <c r="C58" s="19" t="s">
@@ -4628,7 +4680,7 @@
       <c r="AF58" s="27"/>
       <c r="AG58" s="27"/>
     </row>
-    <row r="59" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" s="36"/>
       <c r="B59" s="17"/>
       <c r="C59" s="19" t="s">
@@ -4675,7 +4727,7 @@
       <c r="AF59" s="27"/>
       <c r="AG59" s="27"/>
     </row>
-    <row r="60" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="36"/>
       <c r="B60" s="17"/>
       <c r="C60" s="19" t="s">
@@ -4718,7 +4770,7 @@
       <c r="AF60" s="27"/>
       <c r="AG60" s="27"/>
     </row>
-    <row r="61" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" s="36"/>
       <c r="B61" s="17"/>
       <c r="C61" s="19" t="s">
@@ -4761,7 +4813,7 @@
       <c r="AF61" s="27"/>
       <c r="AG61" s="27"/>
     </row>
-    <row r="62" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="36"/>
       <c r="B62" s="17"/>
       <c r="C62" s="19" t="s">
@@ -4804,7 +4856,7 @@
       <c r="AF62" s="27"/>
       <c r="AG62" s="27"/>
     </row>
-    <row r="63" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63" s="36"/>
       <c r="B63" s="17"/>
       <c r="C63" s="19" t="s">
@@ -4847,7 +4899,7 @@
       <c r="AF63" s="27"/>
       <c r="AG63" s="27"/>
     </row>
-    <row r="64" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="36"/>
       <c r="B64" s="17"/>
       <c r="C64" s="19" t="s">
@@ -4890,7 +4942,7 @@
       <c r="AF64" s="27"/>
       <c r="AG64" s="27"/>
     </row>
-    <row r="65" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65" s="36"/>
       <c r="B65" s="17"/>
       <c r="C65" s="19" t="s">
@@ -4933,7 +4985,7 @@
       <c r="AF65" s="27"/>
       <c r="AG65" s="27"/>
     </row>
-    <row r="66" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66" s="36"/>
       <c r="B66" s="17"/>
       <c r="C66" s="19" t="s">
@@ -4978,7 +5030,7 @@
       <c r="AF66" s="27"/>
       <c r="AG66" s="27"/>
     </row>
-    <row r="67" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67" s="36"/>
       <c r="B67" s="17"/>
       <c r="C67" s="19" t="s">
@@ -5025,7 +5077,7 @@
       <c r="AF67" s="27"/>
       <c r="AG67" s="27"/>
     </row>
-    <row r="68" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68" s="36"/>
       <c r="B68" s="17"/>
       <c r="C68" s="19" t="s">
@@ -5132,18 +5184,16 @@
       <c r="AC70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD70" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE70" s="14" t="s">
+      <c r="AD70" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE70" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF70" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG70" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="AG70" s="26"/>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71" s="32"/>
@@ -5203,18 +5253,16 @@
       <c r="AC71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AD71" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE71" s="14" t="s">
+      <c r="AD71" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE71" s="26" t="s">
         <v>55</v>
       </c>
       <c r="AF71" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AG71" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="AG71" s="26"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72" s="32"/>
@@ -5274,12 +5322,12 @@
       <c r="AC72" s="26">
         <v>4</v>
       </c>
-      <c r="AD72" s="14"/>
-      <c r="AE72" s="14"/>
+      <c r="AD72" s="26"/>
+      <c r="AE72" s="26"/>
       <c r="AF72" s="26">
         <v>4</v>
       </c>
-      <c r="AG72" s="14"/>
+      <c r="AG72" s="26"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73" s="32"/>
@@ -5339,16 +5387,16 @@
       <c r="AC73" s="26">
         <v>5</v>
       </c>
-      <c r="AD73" s="14">
+      <c r="AD73" s="26">
         <v>4</v>
       </c>
-      <c r="AE73" s="14">
+      <c r="AE73" s="26">
         <v>4</v>
       </c>
       <c r="AF73" s="26">
         <v>5</v>
       </c>
-      <c r="AG73" s="14"/>
+      <c r="AG73" s="26"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74" s="32"/>
@@ -5386,12 +5434,12 @@
       <c r="AA74" s="26"/>
       <c r="AB74" s="26"/>
       <c r="AC74" s="26"/>
-      <c r="AD74" s="14">
+      <c r="AD74" s="26">
         <v>5</v>
       </c>
-      <c r="AE74" s="14"/>
+      <c r="AE74" s="26"/>
       <c r="AF74" s="26"/>
-      <c r="AG74" s="14"/>
+      <c r="AG74" s="26"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
@@ -5435,10 +5483,10 @@
       <c r="AC75" s="26">
         <v>9</v>
       </c>
-      <c r="AD75" s="14"/>
-      <c r="AE75" s="14"/>
+      <c r="AD75" s="26"/>
+      <c r="AE75" s="26"/>
       <c r="AF75" s="26"/>
-      <c r="AG75" s="14"/>
+      <c r="AG75" s="26"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76" s="32"/>
@@ -5480,10 +5528,10 @@
       <c r="AC76" s="26">
         <v>11</v>
       </c>
-      <c r="AD76" s="14"/>
-      <c r="AE76" s="14"/>
+      <c r="AD76" s="26"/>
+      <c r="AE76" s="26"/>
       <c r="AF76" s="26"/>
-      <c r="AG76" s="14"/>
+      <c r="AG76" s="26"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77" s="32"/>
@@ -5525,10 +5573,10 @@
       <c r="AC77" s="26">
         <v>12</v>
       </c>
-      <c r="AD77" s="14"/>
-      <c r="AE77" s="14"/>
+      <c r="AD77" s="26"/>
+      <c r="AE77" s="26"/>
       <c r="AF77" s="26"/>
-      <c r="AG77" s="14"/>
+      <c r="AG77" s="26"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78" s="32"/>
@@ -5568,10 +5616,10 @@
       <c r="AA78" s="26"/>
       <c r="AB78" s="26"/>
       <c r="AC78" s="26"/>
-      <c r="AD78" s="14"/>
-      <c r="AE78" s="14"/>
+      <c r="AD78" s="26"/>
+      <c r="AE78" s="26"/>
       <c r="AF78" s="26"/>
-      <c r="AG78" s="14"/>
+      <c r="AG78" s="26"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79" s="32"/>
@@ -5611,10 +5659,10 @@
       <c r="AA79" s="26"/>
       <c r="AB79" s="26"/>
       <c r="AC79" s="26"/>
-      <c r="AD79" s="14"/>
-      <c r="AE79" s="14"/>
+      <c r="AD79" s="26"/>
+      <c r="AE79" s="26"/>
       <c r="AF79" s="26"/>
-      <c r="AG79" s="14"/>
+      <c r="AG79" s="26"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80" s="32"/>
@@ -5654,10 +5702,10 @@
       <c r="AA80" s="26"/>
       <c r="AB80" s="26"/>
       <c r="AC80" s="26"/>
-      <c r="AD80" s="14"/>
-      <c r="AE80" s="14"/>
+      <c r="AD80" s="26"/>
+      <c r="AE80" s="26"/>
       <c r="AF80" s="26"/>
-      <c r="AG80" s="14"/>
+      <c r="AG80" s="26"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81" s="33"/>
@@ -5697,12 +5745,12 @@
       <c r="AA81" s="26"/>
       <c r="AB81" s="26"/>
       <c r="AC81" s="26"/>
-      <c r="AD81" s="14"/>
-      <c r="AE81" s="14"/>
+      <c r="AD81" s="26"/>
+      <c r="AE81" s="26"/>
       <c r="AF81" s="26"/>
-      <c r="AG81" s="14"/>
-    </row>
-    <row r="83" spans="1:33" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG81" s="26"/>
+    </row>
+    <row r="83" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>67</v>
       </c>
@@ -5749,7 +5797,7 @@
       <c r="AF83" s="27"/>
       <c r="AG83" s="27"/>
     </row>
-    <row r="84" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84" s="30"/>
       <c r="B84" s="25" t="s">
         <v>96</v>
@@ -5794,7 +5842,7 @@
       <c r="AF84" s="27"/>
       <c r="AG84" s="27"/>
     </row>
-    <row r="85" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85" s="30"/>
       <c r="B85" s="12"/>
       <c r="C85" s="19" t="s">
@@ -5835,7 +5883,7 @@
       <c r="AF85" s="27"/>
       <c r="AG85" s="27"/>
     </row>
-    <row r="86" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" s="30"/>
       <c r="B86" s="12"/>
       <c r="C86" s="19" t="s">
@@ -5876,7 +5924,7 @@
       <c r="AF86" s="27"/>
       <c r="AG86" s="27"/>
     </row>
-    <row r="87" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87" s="30"/>
       <c r="B87" s="12"/>
       <c r="C87" s="19" t="s">
@@ -5939,10 +5987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6528,7 +6576,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>210</v>
+        <v>284</v>
       </c>
       <c r="C41" t="s">
         <v>208</v>
@@ -6542,10 +6590,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C42" t="s">
         <v>211</v>
-      </c>
-      <c r="C42" t="s">
-        <v>212</v>
       </c>
       <c r="D42" t="s">
         <v>111</v>
@@ -6556,10 +6604,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" t="s">
         <v>213</v>
-      </c>
-      <c r="C43" t="s">
-        <v>214</v>
       </c>
       <c r="D43" t="s">
         <v>111</v>
@@ -6570,13 +6618,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C44" t="s">
         <v>216</v>
       </c>
-      <c r="C44" t="s">
-        <v>217</v>
-      </c>
       <c r="D44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6584,13 +6632,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6598,10 +6646,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D46" t="s">
         <v>111</v>
@@ -6612,13 +6660,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" t="s">
         <v>221</v>
-      </c>
-      <c r="C47" t="s">
-        <v>223</v>
-      </c>
-      <c r="D47" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -6626,10 +6674,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D48" t="s">
         <v>111</v>
@@ -6640,10 +6688,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D49" t="s">
         <v>111</v>
@@ -6654,10 +6702,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D50" t="s">
         <v>111</v>
@@ -6668,10 +6716,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D51" t="s">
         <v>111</v>
@@ -6682,7 +6730,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C52" t="s">
         <v>199</v>
@@ -6696,10 +6744,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" t="s">
         <v>233</v>
-      </c>
-      <c r="C53" t="s">
-        <v>234</v>
       </c>
       <c r="D53" t="s">
         <v>111</v>
@@ -6710,10 +6758,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D54" t="s">
         <v>111</v>
@@ -6724,10 +6772,10 @@
         <v>53</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D55" t="s">
         <v>111</v>
@@ -6738,10 +6786,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D56" t="s">
         <v>111</v>
@@ -6752,10 +6800,10 @@
         <v>55</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D57" t="s">
         <v>111</v>
@@ -6766,7 +6814,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C58" t="s">
         <v>111</v>
@@ -6780,10 +6828,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D59" t="s">
         <v>111</v>
@@ -6794,10 +6842,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D60" t="s">
         <v>111</v>
@@ -6808,10 +6856,10 @@
         <v>59</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C61" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D61" t="s">
         <v>111</v>
@@ -6822,10 +6870,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D62" t="s">
         <v>111</v>
@@ -6836,10 +6884,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D63" t="s">
         <v>111</v>
@@ -6850,10 +6898,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C64" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D64" t="s">
         <v>111</v>
@@ -6864,10 +6912,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D65" t="s">
         <v>111</v>
@@ -6878,10 +6926,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C66" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D66" t="s">
         <v>111</v>
@@ -6892,10 +6940,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D67" t="s">
         <v>111</v>
@@ -6906,10 +6954,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
@@ -6920,12 +6968,152 @@
         <v>67</v>
       </c>
       <c r="B69" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="C69" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C70" t="s">
+        <v>267</v>
+      </c>
+      <c r="D70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C71" t="s">
+        <v>268</v>
+      </c>
+      <c r="D71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C72" t="s">
+        <v>270</v>
+      </c>
+      <c r="D72" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C73" t="s">
+        <v>272</v>
+      </c>
+      <c r="D73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C74" t="s">
+        <v>274</v>
+      </c>
+      <c r="D74" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="C75" t="s">
+        <v>276</v>
+      </c>
+      <c r="D75" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C76" t="s">
+        <v>280</v>
+      </c>
+      <c r="D76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="C77" t="s">
+        <v>279</v>
+      </c>
+      <c r="D77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="C78" t="s">
+        <v>282</v>
+      </c>
+      <c r="D78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>283</v>
+      </c>
+      <c r="C79" t="s">
+        <v>285</v>
+      </c>
+      <c r="D79" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Main with 370 users.
</commit_message>
<xml_diff>
--- a/MODELO BD COLCIENCIAS UAPA.xlsx
+++ b/MODELO BD COLCIENCIAS UAPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EA89AC-684E-4746-9365-4628FB46E84F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15DA34F-839F-4B7E-AAFD-6E5D00458779}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6630" xr2:uid="{5E1B666F-456F-4C9B-87BC-E270A41FB342}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="312">
   <si>
     <t>JURADO_COMITES</t>
   </si>
@@ -960,6 +960,9 @@
   </si>
   <si>
     <t>Jurado Doctorado</t>
+  </si>
+  <si>
+    <t>Datos complementarios - Jurado/Comisiones evaluadoras de trabajo de grado - Otra</t>
   </si>
 </sst>
 </file>
@@ -1686,10 +1689,10 @@
   <dimension ref="A1:AG87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26:F31"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6075,10 +6078,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8806AF1F-FDC5-4CAC-947D-AB233541C4B7}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7371,6 +7374,11 @@
       </c>
       <c r="D91" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>